<commit_message>
add two scenarios--more/very financially constrained firms
add two scenarios--more/very financially constrained firms
</commit_message>
<xml_diff>
--- a/model/scenario_stack.xlsx
+++ b/model/scenario_stack.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27510"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>alpha</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>debt recov2</t>
+  </si>
+  <si>
+    <t>iota1</t>
+  </si>
+  <si>
+    <t>iota2</t>
   </si>
 </sst>
 </file>
@@ -4938,13 +4944,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:Y51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4952,17 +4958,17 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="10.83203125" style="9"/>
     <col min="3" max="3" width="10.83203125" style="11"/>
-    <col min="4" max="11" width="10.83203125" style="14"/>
-    <col min="12" max="12" width="10.83203125" style="8"/>
-    <col min="13" max="15" width="10.83203125" style="5"/>
-    <col min="16" max="18" width="10.83203125" style="40"/>
-    <col min="19" max="19" width="10.83203125" style="10"/>
-    <col min="20" max="20" width="10.83203125" style="16"/>
-    <col min="21" max="22" width="10.83203125" style="35"/>
-    <col min="23" max="16384" width="10.83203125" style="3"/>
+    <col min="4" max="13" width="10.83203125" style="14"/>
+    <col min="14" max="14" width="10.83203125" style="8"/>
+    <col min="15" max="17" width="10.83203125" style="5"/>
+    <col min="18" max="20" width="10.83203125" style="40"/>
+    <col min="21" max="21" width="10.83203125" style="10"/>
+    <col min="22" max="22" width="10.83203125" style="16"/>
+    <col min="23" max="24" width="10.83203125" style="35"/>
+    <col min="25" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -4996,41 +5002,47 @@
       <c r="K1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="R1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="S1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="T1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="W1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="X1" s="27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="60">
         <v>1</v>
       </c>
@@ -5064,45 +5076,51 @@
       <c r="K2" s="62">
         <v>0.7</v>
       </c>
-      <c r="L2" s="63">
+      <c r="L2" s="62">
+        <v>0.03</v>
+      </c>
+      <c r="M2" s="62">
+        <v>0.01</v>
+      </c>
+      <c r="N2" s="63">
         <v>3.944565522E-2</v>
       </c>
-      <c r="M2" s="64">
+      <c r="O2" s="64">
         <v>3.7795549754999998E-2</v>
       </c>
-      <c r="N2" s="64">
+      <c r="P2" s="64">
         <v>1.8851469270050001</v>
       </c>
-      <c r="O2" s="64">
+      <c r="Q2" s="64">
         <v>1.6052439952290001</v>
       </c>
-      <c r="P2" s="65">
+      <c r="R2" s="65">
         <v>39.395178165163003</v>
       </c>
-      <c r="Q2" s="66">
+      <c r="S2" s="66">
         <v>2.5846971547109998</v>
       </c>
-      <c r="R2" s="66">
+      <c r="T2" s="66">
         <v>3.303589746094</v>
       </c>
-      <c r="S2" s="33">
+      <c r="U2" s="33">
         <v>3.152356756933</v>
       </c>
-      <c r="T2" s="34">
+      <c r="V2" s="34">
         <v>0.35118819705299997</v>
       </c>
-      <c r="U2" s="38">
+      <c r="W2" s="38">
         <v>0.49486251781599999</v>
       </c>
-      <c r="V2" s="38">
+      <c r="X2" s="38">
         <v>0.63374244784900002</v>
       </c>
-      <c r="W2" s="38">
-        <f t="shared" ref="W2" si="0">AVERAGE(U2:V2)</f>
+      <c r="Y2" s="38">
+        <f t="shared" ref="Y2" si="0">AVERAGE(W2:X2)</f>
         <v>0.56430248283250006</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -5136,41 +5154,47 @@
       <c r="K3" s="14">
         <v>0.7</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M3" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N3" s="8">
         <v>4.0932188103999997E-2</v>
       </c>
-      <c r="M3" s="5">
+      <c r="O3" s="5">
         <v>3.8846510926E-2</v>
       </c>
-      <c r="N3" s="5">
+      <c r="P3" s="5">
         <v>1.8694478353549999</v>
       </c>
-      <c r="O3" s="5">
+      <c r="Q3" s="5">
         <v>1.5969558254930001</v>
       </c>
-      <c r="P3" s="54">
+      <c r="R3" s="54">
         <v>25.492519462370002</v>
       </c>
-      <c r="Q3" s="45">
+      <c r="S3" s="45">
         <v>1.7746131608639999</v>
       </c>
-      <c r="R3" s="45">
+      <c r="T3" s="45">
         <v>2.2501230468750002</v>
       </c>
-      <c r="S3" s="10">
+      <c r="U3" s="10">
         <v>3.4125259358090001</v>
       </c>
-      <c r="T3" s="16">
+      <c r="V3" s="16">
         <v>0.33499650927899999</v>
       </c>
-      <c r="U3" s="35">
+      <c r="W3" s="35">
         <v>0.47973497192699999</v>
       </c>
-      <c r="V3" s="35">
+      <c r="X3" s="35">
         <v>0.61342344811600003</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -5204,42 +5228,48 @@
       <c r="K4" s="14">
         <v>0.7</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M4" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N4" s="8">
         <v>4.3104995221000003E-2</v>
       </c>
-      <c r="M4" s="5">
+      <c r="O4" s="5">
         <v>4.0304096934999999E-2</v>
       </c>
-      <c r="N4" s="5">
+      <c r="P4" s="5">
         <v>1.8448434200370001</v>
       </c>
-      <c r="O4" s="5">
+      <c r="Q4" s="5">
         <v>1.5814652817779999</v>
       </c>
-      <c r="P4" s="54">
+      <c r="R4" s="54">
         <v>12.794731455542999</v>
       </c>
-      <c r="Q4" s="45">
+      <c r="S4" s="45">
         <v>0.99746713955999999</v>
       </c>
-      <c r="R4" s="45">
+      <c r="T4" s="45">
         <v>1.2826068749999999</v>
       </c>
-      <c r="S4" s="10">
+      <c r="U4" s="10">
         <v>3.9182129093540001</v>
       </c>
-      <c r="T4" s="16">
+      <c r="V4" s="16">
         <v>0.31083755945399999</v>
       </c>
-      <c r="U4" s="35">
+      <c r="W4" s="35">
         <v>0.45048001748799998</v>
       </c>
-      <c r="V4" s="35">
+      <c r="X4" s="35">
         <v>0.57558064194199998</v>
       </c>
-      <c r="W4" s="3"/>
-    </row>
-    <row r="5" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y4" s="3"/>
+    </row>
+    <row r="5" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -5273,42 +5303,48 @@
       <c r="K5" s="14">
         <v>0.7</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M5" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N5" s="8">
         <v>4.4678860000999999E-2</v>
       </c>
-      <c r="M5" s="5">
+      <c r="O5" s="5">
         <v>4.1269926656000003E-2</v>
       </c>
-      <c r="N5" s="5">
+      <c r="P5" s="5">
         <v>1.8265284136490001</v>
       </c>
-      <c r="O5" s="5">
+      <c r="Q5" s="5">
         <v>1.5711938480859999</v>
       </c>
-      <c r="P5" s="54">
+      <c r="R5" s="54">
         <v>7.1798474483939998</v>
       </c>
-      <c r="Q5" s="45">
+      <c r="S5" s="45">
         <v>0.63143750683199995</v>
       </c>
-      <c r="R5" s="45">
+      <c r="T5" s="45">
         <v>0.81620437499999998</v>
       </c>
-      <c r="S5" s="10">
+      <c r="U5" s="10">
         <v>4.548712572316</v>
       </c>
-      <c r="T5" s="16">
+      <c r="V5" s="16">
         <v>0.28814579237600002</v>
       </c>
-      <c r="U5" s="35">
+      <c r="W5" s="35">
         <v>0.41894258414899999</v>
       </c>
-      <c r="V5" s="35">
+      <c r="X5" s="35">
         <v>0.53458498071299998</v>
       </c>
-      <c r="W5" s="3"/>
-    </row>
-    <row r="6" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y5" s="3"/>
+    </row>
+    <row r="6" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -5342,42 +5378,48 @@
       <c r="K6" s="14">
         <v>0.7</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M6" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N6" s="8">
         <v>4.5476535326000003E-2</v>
       </c>
-      <c r="M6" s="5">
+      <c r="O6" s="5">
         <v>4.1582273910000002E-2</v>
       </c>
-      <c r="N6" s="5">
+      <c r="P6" s="5">
         <v>1.8146394792889999</v>
       </c>
-      <c r="O6" s="5">
+      <c r="Q6" s="5">
         <v>1.565814330199</v>
       </c>
-      <c r="P6" s="54">
+      <c r="R6" s="54">
         <v>4.3577916756199997</v>
       </c>
-      <c r="Q6" s="45">
+      <c r="S6" s="45">
         <v>0.43338588776999998</v>
       </c>
-      <c r="R6" s="45">
+      <c r="T6" s="45">
         <v>0.5625</v>
       </c>
-      <c r="S6" s="10">
+      <c r="U6" s="10">
         <v>5.3304240251800001</v>
       </c>
-      <c r="T6" s="16">
+      <c r="V6" s="16">
         <v>0.26663591236299999</v>
       </c>
-      <c r="U6" s="35">
+      <c r="W6" s="35">
         <v>0.386644167195</v>
       </c>
-      <c r="V6" s="35">
+      <c r="X6" s="35">
         <v>0.492767923936</v>
       </c>
-      <c r="W6" s="3"/>
-    </row>
-    <row r="7" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y6" s="3"/>
+    </row>
+    <row r="7" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -5411,42 +5453,48 @@
       <c r="K7" s="14">
         <v>0.7</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M7" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N7" s="8">
         <v>4.5552263508999997E-2</v>
       </c>
-      <c r="M7" s="5">
+      <c r="O7" s="5">
         <v>4.1294445988E-2</v>
       </c>
-      <c r="N7" s="5">
+      <c r="P7" s="5">
         <v>1.800445214757</v>
       </c>
-      <c r="O7" s="5">
+      <c r="Q7" s="5">
         <v>1.5593876982029999</v>
       </c>
-      <c r="P7" s="54">
+      <c r="R7" s="54">
         <v>2.792443562316</v>
       </c>
-      <c r="Q7" s="45">
+      <c r="S7" s="45">
         <v>0.31565818079699998</v>
       </c>
-      <c r="R7" s="45">
+      <c r="T7" s="45">
         <v>0.41625000000000001</v>
       </c>
-      <c r="S7" s="10">
+      <c r="U7" s="10">
         <v>6.2812799682799998</v>
       </c>
-      <c r="T7" s="16">
+      <c r="V7" s="16">
         <v>0.24746451646500001</v>
       </c>
-      <c r="U7" s="35">
+      <c r="W7" s="35">
         <v>0.35351982069600002</v>
       </c>
-      <c r="V7" s="35">
+      <c r="X7" s="35">
         <v>0.45055831256399997</v>
       </c>
-      <c r="W7" s="3"/>
-    </row>
-    <row r="8" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y7" s="3"/>
+    </row>
+    <row r="8" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -5480,42 +5528,48 @@
       <c r="K8" s="14">
         <v>0.7</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M8" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N8" s="8">
         <v>4.4542787703999998E-2</v>
       </c>
-      <c r="M8" s="5">
+      <c r="O8" s="5">
         <v>4.0085320516999999E-2</v>
       </c>
-      <c r="N8" s="5">
+      <c r="P8" s="5">
         <v>1.7989776317299999</v>
       </c>
-      <c r="O8" s="5">
+      <c r="Q8" s="5">
         <v>1.5617348645860001</v>
       </c>
-      <c r="P8" s="54">
+      <c r="R8" s="54">
         <v>1.8606531459960001</v>
       </c>
-      <c r="Q8" s="45">
+      <c r="S8" s="45">
         <v>0.23749539650000001</v>
       </c>
-      <c r="R8" s="45">
+      <c r="T8" s="45">
         <v>0.30937500000000001</v>
       </c>
-      <c r="S8" s="10">
+      <c r="U8" s="10">
         <v>7.6150974591020004</v>
       </c>
-      <c r="T8" s="16">
+      <c r="V8" s="16">
         <v>0.22458754249099999</v>
       </c>
-      <c r="U8" s="35">
+      <c r="W8" s="35">
         <v>0.321766462586</v>
       </c>
-      <c r="V8" s="35">
+      <c r="X8" s="35">
         <v>0.40918434263199999</v>
       </c>
-      <c r="W8" s="3"/>
-    </row>
-    <row r="9" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y8" s="3"/>
+    </row>
+    <row r="9" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -5549,42 +5603,48 @@
       <c r="K9" s="14">
         <v>0.7</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M9" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N9" s="8">
         <v>4.3903284793999998E-2</v>
       </c>
-      <c r="M9" s="5">
+      <c r="O9" s="5">
         <v>3.9255656462999999E-2</v>
       </c>
-      <c r="N9" s="5">
+      <c r="P9" s="5">
         <v>1.802362538313</v>
       </c>
-      <c r="O9" s="5">
+      <c r="Q9" s="5">
         <v>1.563919631923</v>
       </c>
-      <c r="P9" s="54">
+      <c r="R9" s="54">
         <v>1.2636724066180001</v>
       </c>
-      <c r="Q9" s="45">
+      <c r="S9" s="45">
         <v>0.18995049326800001</v>
       </c>
-      <c r="R9" s="45">
+      <c r="T9" s="45">
         <v>0.25468750000000001</v>
       </c>
-      <c r="S9" s="10">
+      <c r="U9" s="10">
         <v>9.2254571222490007</v>
       </c>
-      <c r="T9" s="16">
+      <c r="V9" s="16">
         <v>0.21029364670600001</v>
       </c>
-      <c r="U9" s="35">
+      <c r="W9" s="35">
         <v>0.28336196021400001</v>
       </c>
-      <c r="V9" s="35">
+      <c r="X9" s="35">
         <v>0.36093656848599998</v>
       </c>
-      <c r="W9" s="3"/>
-    </row>
-    <row r="10" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y9" s="3"/>
+    </row>
+    <row r="10" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -5618,42 +5678,48 @@
       <c r="K10" s="14">
         <v>0.7</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M10" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N10" s="8">
         <v>4.1866917618000002E-2</v>
       </c>
-      <c r="M10" s="5">
+      <c r="O10" s="5">
         <v>3.7229346342000001E-2</v>
       </c>
-      <c r="N10" s="5">
+      <c r="P10" s="5">
         <v>1.8148014764710001</v>
       </c>
-      <c r="O10" s="5">
+      <c r="Q10" s="5">
         <v>1.5755587415979999</v>
       </c>
-      <c r="P10" s="54">
+      <c r="R10" s="54">
         <v>0.86748411720499996</v>
       </c>
-      <c r="Q10" s="45">
+      <c r="S10" s="45">
         <v>0.15225495078500001</v>
       </c>
-      <c r="R10" s="45">
+      <c r="T10" s="45">
         <v>0.20250000000000001</v>
       </c>
-      <c r="S10" s="10">
+      <c r="U10" s="10">
         <v>11.692704957553</v>
       </c>
-      <c r="T10" s="16">
+      <c r="V10" s="16">
         <v>0.189942459398</v>
       </c>
-      <c r="U10" s="35">
+      <c r="W10" s="35">
         <v>0.247769231113</v>
       </c>
-      <c r="V10" s="35">
+      <c r="X10" s="35">
         <v>0.31510016717900002</v>
       </c>
-      <c r="W10" s="3"/>
-    </row>
-    <row r="11" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y10" s="3"/>
+    </row>
+    <row r="11" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -5687,42 +5753,48 @@
       <c r="K11" s="14">
         <v>0.7</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M11" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N11" s="8">
         <v>3.9484584091000002E-2</v>
       </c>
-      <c r="M11" s="5">
+      <c r="O11" s="5">
         <v>3.4940077751999997E-2</v>
       </c>
-      <c r="N11" s="5">
+      <c r="P11" s="5">
         <v>1.8289295610580001</v>
       </c>
-      <c r="O11" s="5">
+      <c r="Q11" s="5">
         <v>1.5884386079899999</v>
       </c>
-      <c r="P11" s="54">
+      <c r="R11" s="54">
         <v>0.58383821946199999</v>
       </c>
-      <c r="Q11" s="45">
+      <c r="S11" s="45">
         <v>0.12541903074399999</v>
       </c>
-      <c r="R11" s="45">
+      <c r="T11" s="45">
         <v>0.17249999999999999</v>
       </c>
-      <c r="S11" s="10">
+      <c r="U11" s="10">
         <v>15.183569526095001</v>
       </c>
-      <c r="T11" s="16">
+      <c r="V11" s="16">
         <v>0.17476194475500001</v>
       </c>
-      <c r="U11" s="35">
+      <c r="W11" s="35">
         <v>0.20703646349900001</v>
       </c>
-      <c r="V11" s="35">
+      <c r="X11" s="35">
         <v>0.264101917686</v>
       </c>
-      <c r="W11" s="3"/>
-    </row>
-    <row r="12" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y11" s="3"/>
+    </row>
+    <row r="12" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -5756,42 +5828,48 @@
       <c r="K12" s="14">
         <v>0.7</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M12" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N12" s="8">
         <v>3.6201238333999998E-2</v>
       </c>
-      <c r="M12" s="5">
+      <c r="O12" s="5">
         <v>3.1899911333999997E-2</v>
       </c>
-      <c r="N12" s="5">
+      <c r="P12" s="5">
         <v>1.866147310603</v>
       </c>
-      <c r="O12" s="5">
+      <c r="Q12" s="5">
         <v>1.61730190536</v>
       </c>
-      <c r="P12" s="54">
+      <c r="R12" s="54">
         <v>0.38047046413699998</v>
       </c>
-      <c r="Q12" s="45">
+      <c r="S12" s="45">
         <v>0.10352876997300001</v>
       </c>
-      <c r="R12" s="45">
+      <c r="T12" s="45">
         <v>0.14249999999999999</v>
       </c>
-      <c r="S12" s="10">
+      <c r="U12" s="10">
         <v>21.334731210087</v>
       </c>
-      <c r="T12" s="16">
+      <c r="V12" s="16">
         <v>0.15572603086</v>
       </c>
-      <c r="U12" s="35">
+      <c r="W12" s="35">
         <v>0.165373325189</v>
       </c>
-      <c r="V12" s="35">
+      <c r="X12" s="35">
         <v>0.21092970424999999</v>
       </c>
-      <c r="W12" s="3"/>
-    </row>
-    <row r="13" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y12" s="3"/>
+    </row>
+    <row r="13" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -5825,42 +5903,48 @@
       <c r="K13" s="14">
         <v>0.7</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M13" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N13" s="8">
         <v>3.2263753519000002E-2</v>
       </c>
-      <c r="M13" s="5">
+      <c r="O13" s="5">
         <v>2.8324930068E-2</v>
       </c>
-      <c r="N13" s="5">
+      <c r="P13" s="5">
         <v>1.9277793332549999</v>
       </c>
-      <c r="O13" s="5">
+      <c r="Q13" s="5">
         <v>1.652491340533</v>
       </c>
-      <c r="P13" s="54">
+      <c r="R13" s="54">
         <v>0.22461361807999999</v>
       </c>
-      <c r="Q13" s="45">
+      <c r="S13" s="45">
         <v>8.6128947459999994E-2</v>
       </c>
-      <c r="R13" s="45">
+      <c r="T13" s="45">
         <v>0.121875</v>
       </c>
-      <c r="S13" s="10">
+      <c r="U13" s="10">
         <v>33.424434231896001</v>
       </c>
-      <c r="T13" s="16">
+      <c r="V13" s="16">
         <v>0.138763013776</v>
       </c>
-      <c r="U13" s="35">
+      <c r="W13" s="35">
         <v>0.118264843572</v>
       </c>
-      <c r="V13" s="35">
+      <c r="X13" s="35">
         <v>0.15137984268599999</v>
       </c>
-      <c r="W13" s="3"/>
-    </row>
-    <row r="14" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y13" s="3"/>
+    </row>
+    <row r="14" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -5894,42 +5978,48 @@
       <c r="K14" s="14">
         <v>0.7</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L14" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M14" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N14" s="8">
         <v>3.7936109448000001E-2</v>
       </c>
-      <c r="M14" s="5">
+      <c r="O14" s="5">
         <v>3.66891232E-2</v>
       </c>
-      <c r="N14" s="5">
+      <c r="P14" s="5">
         <v>1.9035294688890001</v>
       </c>
-      <c r="O14" s="5">
+      <c r="Q14" s="5">
         <v>1.6184253114560001</v>
       </c>
-      <c r="P14" s="54">
+      <c r="R14" s="54">
         <v>59.804828575518997</v>
       </c>
-      <c r="Q14" s="45">
+      <c r="S14" s="45">
         <v>3.7230679099209998</v>
       </c>
-      <c r="R14" s="45">
+      <c r="T14" s="45">
         <v>4.7457140625000003</v>
       </c>
-      <c r="S14" s="10">
+      <c r="U14" s="10">
         <v>2.9595741228230001</v>
       </c>
-      <c r="T14" s="16">
+      <c r="V14" s="16">
         <v>0.36427885835899998</v>
       </c>
-      <c r="U14" s="35">
+      <c r="W14" s="35">
         <v>0.50792921154500004</v>
       </c>
-      <c r="V14" s="35">
+      <c r="X14" s="35">
         <v>0.65093263635700005</v>
       </c>
-      <c r="W14" s="3"/>
-    </row>
-    <row r="15" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y14" s="3"/>
+    </row>
+    <row r="15" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -5963,42 +6053,48 @@
       <c r="K15" s="14">
         <v>0.7</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L15" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M15" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N15" s="8">
         <v>3.3778703894999998E-2</v>
       </c>
-      <c r="M15" s="5">
+      <c r="O15" s="5">
         <v>3.3511987141000003E-2</v>
       </c>
-      <c r="N15" s="5">
+      <c r="P15" s="5">
         <v>1.943117232791</v>
       </c>
-      <c r="O15" s="5">
+      <c r="Q15" s="5">
         <v>1.6444761029920001</v>
       </c>
-      <c r="P15" s="54">
+      <c r="R15" s="54">
         <v>179.75923863906399</v>
       </c>
-      <c r="Q15" s="45">
+      <c r="S15" s="45">
         <v>9.9347547579820006</v>
       </c>
-      <c r="R15" s="45">
+      <c r="T15" s="45">
         <v>12.4690671875</v>
       </c>
-      <c r="S15" s="10">
+      <c r="U15" s="10">
         <v>2.5954918290040001</v>
       </c>
-      <c r="T15" s="16">
+      <c r="V15" s="16">
         <v>0.392918976147</v>
       </c>
-      <c r="U15" s="35">
+      <c r="W15" s="35">
         <v>0.53659222280800001</v>
       </c>
-      <c r="V15" s="35">
+      <c r="X15" s="35">
         <v>0.68847342359700003</v>
       </c>
-      <c r="W15" s="3"/>
-    </row>
-    <row r="16" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y15" s="3"/>
+    </row>
+    <row r="16" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -6032,42 +6128,48 @@
       <c r="K16" s="14">
         <v>0.7</v>
       </c>
-      <c r="L16" s="8">
+      <c r="L16" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M16" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N16" s="8">
         <v>2.8718286536E-2</v>
       </c>
-      <c r="M16" s="5">
+      <c r="O16" s="5">
         <v>2.9468021659000001E-2</v>
       </c>
-      <c r="N16" s="5">
+      <c r="P16" s="5">
         <v>1.9987838891630001</v>
       </c>
-      <c r="O16" s="5">
+      <c r="Q16" s="5">
         <v>1.680989882832</v>
       </c>
-      <c r="P16" s="54">
+      <c r="R16" s="54">
         <v>801.06005626381602</v>
       </c>
-      <c r="Q16" s="45">
+      <c r="S16" s="45">
         <v>39.290103048340001</v>
       </c>
-      <c r="R16" s="45">
+      <c r="T16" s="45">
         <v>48.901013124999999</v>
       </c>
-      <c r="S16" s="10">
+      <c r="U16" s="10">
         <v>2.2718871417709998</v>
       </c>
-      <c r="T16" s="16">
+      <c r="V16" s="16">
         <v>0.42668940452600002</v>
       </c>
-      <c r="U16" s="35">
+      <c r="W16" s="35">
         <v>0.56385797088599998</v>
       </c>
-      <c r="V16" s="35">
+      <c r="X16" s="35">
         <v>0.72475989826499998</v>
       </c>
-      <c r="W16" s="3"/>
-    </row>
-    <row r="17" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y16" s="3"/>
+    </row>
+    <row r="17" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -6101,42 +6203,48 @@
       <c r="K17" s="14">
         <v>0.7</v>
       </c>
-      <c r="L17" s="8">
+      <c r="L17" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M17" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N17" s="8">
         <v>2.2657744436E-2</v>
       </c>
-      <c r="M17" s="5">
+      <c r="O17" s="5">
         <v>2.4094632961999998E-2</v>
       </c>
-      <c r="N17" s="5">
+      <c r="P17" s="5">
         <v>2.0717829398080001</v>
       </c>
-      <c r="O17" s="5">
+      <c r="Q17" s="5">
         <v>1.7306928825150001</v>
       </c>
-      <c r="P17" s="54">
+      <c r="R17" s="54">
         <v>7066.20553069378</v>
       </c>
-      <c r="Q17" s="45">
+      <c r="S17" s="45">
         <v>305.437928077729</v>
       </c>
-      <c r="R17" s="45">
+      <c r="T17" s="45">
         <v>374.59434687499999</v>
       </c>
-      <c r="S17" s="10">
+      <c r="U17" s="10">
         <v>1.99168472988</v>
       </c>
-      <c r="T17" s="16">
+      <c r="V17" s="16">
         <v>0.46384760378500001</v>
       </c>
-      <c r="U17" s="35">
+      <c r="W17" s="35">
         <v>0.59100635741600005</v>
       </c>
-      <c r="V17" s="35">
+      <c r="X17" s="35">
         <v>0.76099652881299995</v>
       </c>
-      <c r="W17" s="3"/>
-    </row>
-    <row r="18" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y17" s="3"/>
+    </row>
+    <row r="18" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -6170,42 +6278,48 @@
       <c r="K18" s="14">
         <v>0.7</v>
       </c>
-      <c r="L18" s="8">
+      <c r="L18" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M18" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N18" s="8">
         <v>1.5661805147999999E-2</v>
       </c>
-      <c r="M18" s="5">
+      <c r="O18" s="5">
         <v>1.7284008920999998E-2</v>
       </c>
-      <c r="N18" s="5">
+      <c r="P18" s="5">
         <v>2.1771467105740001</v>
       </c>
-      <c r="O18" s="5">
+      <c r="Q18" s="5">
         <v>1.803134432532</v>
       </c>
-      <c r="P18" s="67">
+      <c r="R18" s="67">
         <v>241351.46679388499</v>
       </c>
-      <c r="Q18" s="67">
+      <c r="S18" s="67">
         <v>9100.6254384296099</v>
       </c>
-      <c r="R18" s="67">
+      <c r="T18" s="67">
         <v>11018.073103125</v>
       </c>
-      <c r="S18" s="10">
+      <c r="U18" s="10">
         <v>1.737850166401</v>
       </c>
-      <c r="T18" s="16">
+      <c r="V18" s="16">
         <v>0.50745178317700002</v>
       </c>
-      <c r="U18" s="35">
+      <c r="W18" s="35">
         <v>0.61824560893500002</v>
       </c>
-      <c r="V18" s="35">
+      <c r="X18" s="35">
         <v>0.79782007118200005</v>
       </c>
-      <c r="W18" s="3"/>
-    </row>
-    <row r="19" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y18" s="3"/>
+    </row>
+    <row r="19" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -6239,42 +6353,48 @@
       <c r="K19" s="14">
         <v>0.7</v>
       </c>
-      <c r="L19" s="8">
+      <c r="L19" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M19" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N19" s="8">
         <v>8.2012313290000007E-3</v>
       </c>
-      <c r="M19" s="5">
+      <c r="O19" s="5">
         <v>9.4019975650000004E-3</v>
       </c>
-      <c r="N19" s="5">
+      <c r="P19" s="5">
         <v>2.3489507516189998</v>
       </c>
-      <c r="O19" s="5">
+      <c r="Q19" s="5">
         <v>1.9231542918169999</v>
       </c>
-      <c r="P19" s="67">
+      <c r="R19" s="67">
         <v>235041740.97330201</v>
       </c>
-      <c r="Q19" s="67">
+      <c r="S19" s="67">
         <v>7649432.2719721897</v>
       </c>
-      <c r="R19" s="67">
+      <c r="T19" s="67">
         <v>9072444.8499749899</v>
       </c>
-      <c r="S19" s="10">
+      <c r="U19" s="10">
         <v>1.5064126131810001</v>
       </c>
-      <c r="T19" s="16">
+      <c r="V19" s="16">
         <v>0.56107755596200004</v>
       </c>
-      <c r="U19" s="35">
+      <c r="W19" s="35">
         <v>0.64408495415400002</v>
       </c>
-      <c r="V19" s="35">
+      <c r="X19" s="35">
         <v>0.83309286973200003</v>
       </c>
-      <c r="W19" s="3"/>
-    </row>
-    <row r="20" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y19" s="3"/>
+    </row>
+    <row r="20" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -6308,42 +6428,48 @@
       <c r="K20" s="14">
         <v>0.7</v>
       </c>
-      <c r="L20" s="8">
+      <c r="L20" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M20" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N20" s="8">
         <v>3.5125538519000001E-2</v>
       </c>
-      <c r="M20" s="5">
+      <c r="O20" s="5">
         <v>3.3692745257000001E-2</v>
       </c>
-      <c r="N20" s="5">
+      <c r="P20" s="5">
         <v>1.907925553106</v>
       </c>
-      <c r="O20" s="5">
+      <c r="Q20" s="5">
         <v>1.6213403962649999</v>
       </c>
-      <c r="P20" s="54">
+      <c r="R20" s="54">
         <v>55.657533657240002</v>
       </c>
-      <c r="Q20" s="45">
+      <c r="S20" s="45">
         <v>3.292156188756</v>
       </c>
-      <c r="R20" s="45">
+      <c r="T20" s="45">
         <v>4.1707820543249996</v>
       </c>
-      <c r="S20" s="10">
+      <c r="U20" s="10">
         <v>2.92658113833</v>
       </c>
-      <c r="T20" s="16">
+      <c r="V20" s="16">
         <v>0.36085811807399998</v>
       </c>
-      <c r="U20" s="35">
+      <c r="W20" s="35">
         <v>0.51833628869399995</v>
       </c>
-      <c r="V20" s="35">
+      <c r="X20" s="35">
         <v>0.66469037206500003</v>
       </c>
-      <c r="W20" s="3"/>
-    </row>
-    <row r="21" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="Y20" s="3"/>
+    </row>
+    <row r="21" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -6377,42 +6503,48 @@
       <c r="K21" s="14">
         <v>0.7</v>
       </c>
-      <c r="L21" s="8">
+      <c r="L21" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M21" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N21" s="8">
         <v>3.0062368655000001E-2</v>
       </c>
-      <c r="M21" s="5">
+      <c r="O21" s="5">
         <v>2.8873531107999999E-2</v>
       </c>
-      <c r="N21" s="5">
+      <c r="P21" s="5">
         <v>1.9375060412059999</v>
       </c>
-      <c r="O21" s="5">
+      <c r="Q21" s="5">
         <v>1.640552031211</v>
       </c>
-      <c r="P21" s="54">
+      <c r="R21" s="54">
         <v>83.340410811037003</v>
       </c>
-      <c r="Q21" s="45">
+      <c r="S21" s="45">
         <v>4.3914539552580001</v>
       </c>
-      <c r="R21" s="45">
+      <c r="T21" s="45">
         <v>5.554160260463</v>
       </c>
-      <c r="S21" s="10">
+      <c r="U21" s="10">
         <v>2.684807932819</v>
       </c>
-      <c r="T21" s="16">
+      <c r="V21" s="16">
         <v>0.37402216895700002</v>
       </c>
-      <c r="U21" s="35">
+      <c r="W21" s="35">
         <v>0.54441531409599997</v>
       </c>
-      <c r="V21" s="35">
+      <c r="X21" s="35">
         <v>0.69955715572599997</v>
       </c>
-      <c r="W21" s="3"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Y21" s="3"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -6446,41 +6578,47 @@
       <c r="K22" s="14">
         <v>0.7</v>
       </c>
-      <c r="L22" s="8">
+      <c r="L22" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M22" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N22" s="8">
         <v>2.4123880002000001E-2</v>
       </c>
-      <c r="M22" s="5">
+      <c r="O22" s="5">
         <v>2.3206141435000001E-2</v>
       </c>
-      <c r="N22" s="5">
+      <c r="P22" s="5">
         <v>1.9780765034629999</v>
       </c>
-      <c r="O22" s="5">
+      <c r="Q22" s="5">
         <v>1.667962239085</v>
       </c>
-      <c r="P22" s="54">
+      <c r="R22" s="54">
         <v>135.91729657147599</v>
       </c>
-      <c r="Q22" s="45">
+      <c r="S22" s="45">
         <v>6.2891030649079998</v>
       </c>
-      <c r="R22" s="45">
+      <c r="T22" s="45">
         <v>7.9593749999999996</v>
       </c>
-      <c r="S22" s="10">
+      <c r="U22" s="10">
         <v>2.4306005751119999</v>
       </c>
-      <c r="T22" s="16">
+      <c r="V22" s="16">
         <v>0.39169466331000002</v>
       </c>
-      <c r="U22" s="35">
+      <c r="W22" s="35">
         <v>0.57333615244699998</v>
       </c>
-      <c r="V22" s="35">
+      <c r="X22" s="35">
         <v>0.738472168358</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -6514,41 +6652,47 @@
       <c r="K23" s="14">
         <v>0.7</v>
       </c>
-      <c r="L23" s="8">
+      <c r="L23" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M23" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N23" s="8">
         <v>1.6630933580999999E-2</v>
       </c>
-      <c r="M23" s="5">
+      <c r="O23" s="5">
         <v>1.6031035113999999E-2</v>
       </c>
-      <c r="N23" s="5">
+      <c r="P23" s="5">
         <v>2.0352300632749998</v>
       </c>
-      <c r="O23" s="5">
+      <c r="Q23" s="5">
         <v>1.706646164456</v>
       </c>
-      <c r="P23" s="54">
+      <c r="R23" s="54">
         <v>254.80135388823899</v>
       </c>
-      <c r="Q23" s="45">
+      <c r="S23" s="45">
         <v>9.9893760316049995</v>
       </c>
-      <c r="R23" s="45">
+      <c r="T23" s="45">
         <v>12.581250000000001</v>
       </c>
-      <c r="S23" s="10">
+      <c r="U23" s="10">
         <v>2.1630327501250002</v>
       </c>
-      <c r="T23" s="16">
+      <c r="V23" s="16">
         <v>0.41302221776800002</v>
       </c>
-      <c r="U23" s="35">
+      <c r="W23" s="35">
         <v>0.60995250651900002</v>
       </c>
-      <c r="V23" s="35">
+      <c r="X23" s="35">
         <v>0.78772478100499999</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -6582,41 +6726,47 @@
       <c r="K24" s="14">
         <v>0.7</v>
       </c>
-      <c r="L24" s="8">
+      <c r="L24" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M24" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N24" s="8">
         <v>7.5196853720000002E-3</v>
       </c>
-      <c r="M24" s="5">
+      <c r="O24" s="5">
         <v>7.266812668E-3</v>
       </c>
-      <c r="N24" s="5">
+      <c r="P24" s="5">
         <v>2.1367306718350001</v>
       </c>
-      <c r="O24" s="5">
+      <c r="Q24" s="5">
         <v>1.7789790940529999</v>
       </c>
-      <c r="P24" s="54">
+      <c r="R24" s="54">
         <v>630.45605117503203</v>
       </c>
-      <c r="Q24" s="45">
+      <c r="S24" s="45">
         <v>19.721125825418</v>
       </c>
-      <c r="R24" s="45">
+      <c r="T24" s="45">
         <v>24.609375</v>
       </c>
-      <c r="S24" s="10">
+      <c r="U24" s="10">
         <v>1.860114150532</v>
       </c>
-      <c r="T24" s="16">
+      <c r="V24" s="16">
         <v>0.44317030177200001</v>
       </c>
-      <c r="U24" s="35">
+      <c r="W24" s="35">
         <v>0.65961367831600004</v>
       </c>
-      <c r="V24" s="35">
+      <c r="X24" s="35">
         <v>0.85472065468400005</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -6650,41 +6800,47 @@
       <c r="K25" s="14">
         <v>0.7</v>
       </c>
-      <c r="L25" s="8">
+      <c r="L25" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M25" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N25" s="8">
         <v>4.2755951112E-2</v>
       </c>
-      <c r="M25" s="5">
+      <c r="O25" s="5">
         <v>4.0936288655999999E-2</v>
       </c>
-      <c r="N25" s="5">
+      <c r="P25" s="5">
         <v>1.8667825664269999</v>
       </c>
-      <c r="O25" s="5">
+      <c r="Q25" s="5">
         <v>1.5940558159839999</v>
       </c>
-      <c r="P25" s="54">
+      <c r="R25" s="54">
         <v>29.193780000831001</v>
       </c>
-      <c r="Q25" s="45">
+      <c r="S25" s="45">
         <v>2.0758723456769999</v>
       </c>
-      <c r="R25" s="45">
+      <c r="T25" s="45">
         <v>2.6015769249749998</v>
       </c>
-      <c r="S25" s="10">
+      <c r="U25" s="10">
         <v>3.408508009178</v>
       </c>
-      <c r="T25" s="16">
+      <c r="V25" s="16">
         <v>0.33793758469399998</v>
       </c>
-      <c r="U25" s="35">
+      <c r="W25" s="35">
         <v>0.47657736235800002</v>
       </c>
-      <c r="V25" s="35">
+      <c r="X25" s="35">
         <v>0.60856145395600003</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -6718,41 +6874,47 @@
       <c r="K26" s="14">
         <v>0.7</v>
       </c>
-      <c r="L26" s="8">
+      <c r="L26" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M26" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N26" s="8">
         <v>4.6000933946000001E-2</v>
       </c>
-      <c r="M26" s="5">
+      <c r="O26" s="5">
         <v>4.400989365E-2</v>
       </c>
-      <c r="N26" s="5">
+      <c r="P26" s="5">
         <v>1.854276961876</v>
       </c>
-      <c r="O26" s="5">
+      <c r="Q26" s="5">
         <v>1.587371964111</v>
       </c>
-      <c r="P26" s="54">
+      <c r="R26" s="54">
         <v>22.351885029428999</v>
       </c>
-      <c r="Q26" s="45">
+      <c r="S26" s="45">
         <v>1.7268867014689999</v>
       </c>
-      <c r="R26" s="45">
+      <c r="T26" s="45">
         <v>2.1886282067249998</v>
       </c>
-      <c r="S26" s="10">
+      <c r="U26" s="10">
         <v>3.6144237649159998</v>
       </c>
-      <c r="T26" s="16">
+      <c r="V26" s="16">
         <v>0.33181875327499999</v>
       </c>
-      <c r="U26" s="35">
+      <c r="W26" s="35">
         <v>0.45790248444199999</v>
       </c>
-      <c r="V26" s="35">
+      <c r="X26" s="35">
         <v>0.58425649820299996</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -6786,41 +6948,47 @@
       <c r="K27" s="14">
         <v>0.7</v>
       </c>
-      <c r="L27" s="8">
+      <c r="L27" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M27" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N27" s="8">
         <v>4.8758693882999998E-2</v>
       </c>
-      <c r="M27" s="5">
+      <c r="O27" s="5">
         <v>4.6618128393000002E-2</v>
       </c>
-      <c r="N27" s="5">
+      <c r="P27" s="5">
         <v>1.840644914374</v>
       </c>
-      <c r="O27" s="5">
+      <c r="Q27" s="5">
         <v>1.5795541049490001</v>
       </c>
-      <c r="P27" s="54">
+      <c r="R27" s="54">
         <v>17.529028822992</v>
       </c>
-      <c r="Q27" s="45">
+      <c r="S27" s="45">
         <v>1.461674855004</v>
       </c>
-      <c r="R27" s="45">
+      <c r="T27" s="45">
         <v>1.8582692321250001</v>
       </c>
-      <c r="S27" s="10">
+      <c r="U27" s="10">
         <v>3.8350618083789998</v>
       </c>
-      <c r="T27" s="16">
+      <c r="V27" s="16">
         <v>0.32524432209800003</v>
       </c>
-      <c r="U27" s="35">
+      <c r="W27" s="35">
         <v>0.44061120812100002</v>
       </c>
-      <c r="V27" s="35">
+      <c r="X27" s="35">
         <v>0.56152285060700002</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -6854,41 +7022,47 @@
       <c r="K28" s="14">
         <v>0.7</v>
       </c>
-      <c r="L28" s="8">
+      <c r="L28" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M28" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N28" s="8">
         <v>5.1025624850999998E-2</v>
       </c>
-      <c r="M28" s="5">
+      <c r="O28" s="5">
         <v>4.8760976371999998E-2</v>
       </c>
-      <c r="N28" s="5">
+      <c r="P28" s="5">
         <v>1.8295007022459999</v>
       </c>
-      <c r="O28" s="5">
+      <c r="Q28" s="5">
         <v>1.570517366275</v>
       </c>
-      <c r="P28" s="54">
+      <c r="R28" s="54">
         <v>14.054987417919</v>
       </c>
-      <c r="Q28" s="45">
+      <c r="S28" s="45">
         <v>1.2516801749290001</v>
       </c>
-      <c r="R28" s="45">
+      <c r="T28" s="45">
         <v>1.5795288473060001</v>
       </c>
-      <c r="S28" s="10">
+      <c r="U28" s="10">
         <v>4.0715419285890002</v>
       </c>
-      <c r="T28" s="16">
+      <c r="V28" s="16">
         <v>0.31747649083500001</v>
       </c>
-      <c r="U28" s="35">
+      <c r="W28" s="35">
         <v>0.42570183937400002</v>
       </c>
-      <c r="V28" s="35">
+      <c r="X28" s="35">
         <v>0.54152910642200003</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -6922,41 +7096,47 @@
       <c r="K29" s="14">
         <v>0.7</v>
       </c>
-      <c r="L29" s="8">
+      <c r="L29" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M29" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N29" s="8">
         <v>5.3019316369000001E-2</v>
       </c>
-      <c r="M29" s="5">
+      <c r="O29" s="5">
         <v>5.0644120644E-2</v>
       </c>
-      <c r="N29" s="5">
+      <c r="P29" s="5">
         <v>1.8188438460709999</v>
       </c>
-      <c r="O29" s="5">
+      <c r="Q29" s="5">
         <v>1.564844700416</v>
       </c>
-      <c r="P29" s="54">
+      <c r="R29" s="54">
         <v>11.474521097181</v>
       </c>
-      <c r="Q29" s="45">
+      <c r="S29" s="45">
         <v>1.085713514501</v>
       </c>
-      <c r="R29" s="45">
+      <c r="T29" s="45">
         <v>1.375105</v>
       </c>
-      <c r="S29" s="10">
+      <c r="U29" s="10">
         <v>4.2837596952280004</v>
       </c>
-      <c r="T29" s="16">
+      <c r="V29" s="16">
         <v>0.31184451343199998</v>
       </c>
-      <c r="U29" s="35">
+      <c r="W29" s="35">
         <v>0.41213004118000002</v>
       </c>
-      <c r="V29" s="35">
+      <c r="X29" s="35">
         <v>0.523825187769</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -6990,41 +7170,47 @@
       <c r="K30" s="14">
         <v>0.7</v>
       </c>
-      <c r="L30" s="8">
+      <c r="L30" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M30" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N30" s="8">
         <v>1.0870154809000001E-2</v>
       </c>
-      <c r="M30" s="5">
+      <c r="O30" s="5">
         <v>1.0233214817E-2</v>
       </c>
-      <c r="N30" s="5">
+      <c r="P30" s="5">
         <v>2.0513921041350001</v>
       </c>
-      <c r="O30" s="5">
+      <c r="Q30" s="5">
         <v>1.7251340727390001</v>
       </c>
-      <c r="P30" s="54">
+      <c r="R30" s="54">
         <v>119.641645181225</v>
       </c>
-      <c r="Q30" s="45">
+      <c r="S30" s="45">
         <v>4.115500608904</v>
       </c>
-      <c r="R30" s="45">
+      <c r="T30" s="45">
         <v>5.2131249999999998</v>
       </c>
-      <c r="S30" s="10">
+      <c r="U30" s="10">
         <v>2.1646997366999998</v>
       </c>
-      <c r="T30" s="16">
+      <c r="V30" s="16">
         <v>0.393678212129</v>
       </c>
-      <c r="U30" s="35">
+      <c r="W30" s="35">
         <v>0.63847974731799995</v>
       </c>
-      <c r="V30" s="35">
+      <c r="X30" s="35">
         <v>0.82645957849100005</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -7058,41 +7244,47 @@
       <c r="K31" s="14">
         <v>0.7</v>
       </c>
-      <c r="L31" s="8">
+      <c r="L31" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M31" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N31" s="8">
         <v>5.5379575180000001E-2</v>
       </c>
-      <c r="M31" s="5">
+      <c r="O31" s="5">
         <v>5.1668654783999998E-2</v>
       </c>
-      <c r="N31" s="5">
+      <c r="P31" s="5">
         <v>1.788531748609</v>
       </c>
-      <c r="O31" s="5">
+      <c r="Q31" s="5">
         <v>1.5447759923960001</v>
       </c>
-      <c r="P31" s="54">
+      <c r="R31" s="54">
         <v>4.6269277565899998</v>
       </c>
-      <c r="Q31" s="45">
+      <c r="S31" s="45">
         <v>0.54016855772899997</v>
       </c>
-      <c r="R31" s="45">
+      <c r="T31" s="45">
         <v>0.69</v>
       </c>
-      <c r="S31" s="10">
+      <c r="U31" s="10">
         <v>5.4889693579829997</v>
       </c>
-      <c r="T31" s="16">
+      <c r="V31" s="16">
         <v>0.27892454885399998</v>
       </c>
-      <c r="U31" s="35">
+      <c r="W31" s="35">
         <v>0.360125853404</v>
       </c>
-      <c r="V31" s="35">
+      <c r="X31" s="35">
         <v>0.45666413785299997</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -7126,41 +7318,47 @@
       <c r="K32" s="14">
         <v>0.7</v>
       </c>
-      <c r="L32" s="8">
+      <c r="L32" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M32" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N32" s="8">
         <v>4.584838412E-3</v>
       </c>
-      <c r="M32" s="5">
+      <c r="O32" s="5">
         <v>4.5972564990000003E-3</v>
       </c>
-      <c r="N32" s="5">
+      <c r="P32" s="5">
         <v>2.2518210777140002</v>
       </c>
-      <c r="O32" s="5">
+      <c r="Q32" s="5">
         <v>1.854332485834</v>
       </c>
-      <c r="P32" s="54">
+      <c r="R32" s="54">
         <v>6393.0799960813001</v>
       </c>
-      <c r="Q32" s="45">
+      <c r="S32" s="45">
         <v>184.957508404724</v>
       </c>
-      <c r="R32" s="45">
+      <c r="T32" s="45">
         <v>228.125</v>
       </c>
-      <c r="S32" s="10">
+      <c r="U32" s="10">
         <v>1.6296315490769999</v>
       </c>
-      <c r="T32" s="16">
+      <c r="V32" s="16">
         <v>0.49494919610499999</v>
       </c>
-      <c r="U32" s="35">
+      <c r="W32" s="35">
         <v>0.67367985429300004</v>
       </c>
-      <c r="V32" s="35">
+      <c r="X32" s="35">
         <v>0.87385171414700002</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -7194,44 +7392,1161 @@
       <c r="K33" s="14">
         <v>0.7</v>
       </c>
-      <c r="L33" s="8">
+      <c r="L33" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="M33" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="N33" s="8">
         <v>4.8940829317000001E-2</v>
       </c>
-      <c r="M33" s="5">
+      <c r="O33" s="5">
         <v>4.8313815325000002E-2</v>
       </c>
-      <c r="N33" s="5">
+      <c r="P33" s="5">
         <v>1.864169846542</v>
       </c>
-      <c r="O33" s="5">
+      <c r="Q33" s="5">
         <v>1.5950985338829999</v>
       </c>
-      <c r="P33" s="54">
+      <c r="R33" s="54">
         <v>38.022146954187001</v>
       </c>
-      <c r="Q33" s="45">
+      <c r="S33" s="45">
         <v>2.96462046134</v>
       </c>
-      <c r="R33" s="45">
+      <c r="T33" s="45">
         <v>3.6850000000000001</v>
       </c>
-      <c r="S33" s="10">
+      <c r="U33" s="10">
         <v>3.4180165360960002</v>
       </c>
-      <c r="T33" s="16">
+      <c r="V33" s="16">
         <v>0.34976919320599997</v>
       </c>
-      <c r="U33" s="35">
+      <c r="W33" s="35">
         <v>0.46002764227600002</v>
       </c>
-      <c r="V33" s="35">
+      <c r="X33" s="35">
         <v>0.58576905757300002</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="P34" s="54"/>
-      <c r="Q34" s="45"/>
-      <c r="R34" s="45"/>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C34" s="11">
+        <v>0</v>
+      </c>
+      <c r="D34" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E34" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F34" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G34" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H34" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I34" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J34" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K34" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L34" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="M34" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="N34" s="8">
+        <v>1.0870154809000001E-2</v>
+      </c>
+      <c r="O34" s="5">
+        <v>1.0233214817E-2</v>
+      </c>
+      <c r="P34" s="5">
+        <v>2.0513921041350001</v>
+      </c>
+      <c r="Q34" s="5">
+        <v>1.7251340727390001</v>
+      </c>
+      <c r="R34" s="54">
+        <v>119.641645181225</v>
+      </c>
+      <c r="S34" s="45">
+        <v>4.115500608904</v>
+      </c>
+      <c r="T34" s="45">
+        <v>5.2131249999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C35" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D35" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E35" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F35" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G35" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H35" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I35" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J35" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K35" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L35" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="M35" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="N35" s="8">
+        <v>4.3104995221000003E-2</v>
+      </c>
+      <c r="O35" s="5">
+        <v>4.0304096934999999E-2</v>
+      </c>
+      <c r="P35" s="5">
+        <v>1.8448434200370001</v>
+      </c>
+      <c r="Q35" s="5">
+        <v>1.5814652817779999</v>
+      </c>
+      <c r="R35" s="40">
+        <v>12.794731455542999</v>
+      </c>
+      <c r="S35" s="40">
+        <v>0.99746713955999999</v>
+      </c>
+      <c r="T35" s="40">
+        <v>1.2826068749999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C36" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D36" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E36" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F36" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G36" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H36" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I36" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J36" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K36" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L36" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="M36" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="N36" s="8">
+        <v>5.5379575180000001E-2</v>
+      </c>
+      <c r="O36" s="5">
+        <v>5.1668654783999998E-2</v>
+      </c>
+      <c r="P36" s="5">
+        <v>1.788531748609</v>
+      </c>
+      <c r="Q36" s="5">
+        <v>1.5447759923960001</v>
+      </c>
+      <c r="R36" s="40">
+        <v>4.6269277565899998</v>
+      </c>
+      <c r="S36" s="40">
+        <v>0.54016855772899997</v>
+      </c>
+      <c r="T36" s="40">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="9">
+        <v>0.627</v>
+      </c>
+      <c r="C37" s="11">
+        <v>0</v>
+      </c>
+      <c r="D37" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E37" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F37" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G37" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H37" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I37" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J37" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K37" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L37" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="M37" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="N37" s="8">
+        <v>7.5196853720000002E-3</v>
+      </c>
+      <c r="O37" s="5">
+        <v>7.266812668E-3</v>
+      </c>
+      <c r="P37" s="5">
+        <v>2.1367306718350001</v>
+      </c>
+      <c r="Q37" s="5">
+        <v>1.7789790940529999</v>
+      </c>
+      <c r="R37" s="40">
+        <v>630.45605117503203</v>
+      </c>
+      <c r="S37" s="40">
+        <v>19.721125825418</v>
+      </c>
+      <c r="T37" s="40">
+        <v>24.609375</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="9">
+        <v>0.627</v>
+      </c>
+      <c r="C38" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D38" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E38" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F38" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G38" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H38" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I38" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J38" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K38" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L38" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="M38" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="N38" s="8">
+        <v>3.944565522E-2</v>
+      </c>
+      <c r="O38" s="5">
+        <v>3.7795549754999998E-2</v>
+      </c>
+      <c r="P38" s="5">
+        <v>1.8851469270050001</v>
+      </c>
+      <c r="Q38" s="5">
+        <v>1.6052439952290001</v>
+      </c>
+      <c r="R38" s="40">
+        <v>39.395178165163003</v>
+      </c>
+      <c r="S38" s="40">
+        <v>2.5846971547109998</v>
+      </c>
+      <c r="T38" s="40">
+        <v>3.303589746094</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="9">
+        <v>0.627</v>
+      </c>
+      <c r="C39" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D39" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E39" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F39" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G39" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H39" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I39" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J39" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K39" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L39" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="M39" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="N39" s="8">
+        <v>5.3019316369000001E-2</v>
+      </c>
+      <c r="O39" s="5">
+        <v>5.0644120644E-2</v>
+      </c>
+      <c r="P39" s="5">
+        <v>1.8188438460709999</v>
+      </c>
+      <c r="Q39" s="5">
+        <v>1.564844700416</v>
+      </c>
+      <c r="R39" s="40">
+        <v>11.474521097181</v>
+      </c>
+      <c r="S39" s="40">
+        <v>1.085713514501</v>
+      </c>
+      <c r="T39" s="40">
+        <v>1.375105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C40" s="11">
+        <v>0</v>
+      </c>
+      <c r="D40" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E40" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F40" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G40" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H40" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I40" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J40" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K40" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L40" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="M40" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="N40" s="8">
+        <v>4.584838412E-3</v>
+      </c>
+      <c r="O40" s="5">
+        <v>4.5972564990000003E-3</v>
+      </c>
+      <c r="P40" s="5">
+        <v>2.2518210777140002</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>1.854332485834</v>
+      </c>
+      <c r="R40" s="40">
+        <v>6393.0799960813001</v>
+      </c>
+      <c r="S40" s="40">
+        <v>184.957508404724</v>
+      </c>
+      <c r="T40" s="40">
+        <v>228.125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C41" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D41" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E41" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F41" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G41" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H41" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I41" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J41" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K41" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L41" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="M41" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="N41" s="8">
+        <v>3.3778703894999998E-2</v>
+      </c>
+      <c r="O41" s="5">
+        <v>3.3511987141000003E-2</v>
+      </c>
+      <c r="P41" s="5">
+        <v>1.943117232791</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>1.6444761029920001</v>
+      </c>
+      <c r="R41" s="40">
+        <v>179.75923863906399</v>
+      </c>
+      <c r="S41" s="40">
+        <v>9.9347547579820006</v>
+      </c>
+      <c r="T41" s="40">
+        <v>12.4690671875</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C42" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D42" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E42" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F42" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G42" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H42" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I42" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J42" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K42" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L42" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="M42" s="14">
+        <v>0.03</v>
+      </c>
+      <c r="N42" s="8">
+        <v>4.8940829317000001E-2</v>
+      </c>
+      <c r="O42" s="5">
+        <v>4.8313815325000002E-2</v>
+      </c>
+      <c r="P42" s="5">
+        <v>1.864169846542</v>
+      </c>
+      <c r="Q42" s="5">
+        <v>1.5950985338829999</v>
+      </c>
+      <c r="R42" s="40">
+        <v>38.022146954187001</v>
+      </c>
+      <c r="S42" s="40">
+        <v>2.96462046134</v>
+      </c>
+      <c r="T42" s="40">
+        <v>3.6850000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C43" s="11">
+        <v>0</v>
+      </c>
+      <c r="D43" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E43" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F43" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G43" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H43" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I43" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J43" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K43" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L43" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="M43" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="N43" s="8">
+        <v>1.0870154809000001E-2</v>
+      </c>
+      <c r="O43" s="5">
+        <v>1.0233214817E-2</v>
+      </c>
+      <c r="P43" s="5">
+        <v>2.0513921041350001</v>
+      </c>
+      <c r="Q43" s="5">
+        <v>1.7251340727390001</v>
+      </c>
+      <c r="R43" s="54">
+        <v>119.641645181225</v>
+      </c>
+      <c r="S43" s="45">
+        <v>4.115500608904</v>
+      </c>
+      <c r="T43" s="45">
+        <v>5.2131249999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C44" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D44" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E44" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F44" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G44" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H44" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I44" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J44" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K44" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L44" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="M44" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="N44" s="8">
+        <v>4.3104995221000003E-2</v>
+      </c>
+      <c r="O44" s="5">
+        <v>4.0304096934999999E-2</v>
+      </c>
+      <c r="P44" s="5">
+        <v>1.8448434200370001</v>
+      </c>
+      <c r="Q44" s="5">
+        <v>1.5814652817779999</v>
+      </c>
+      <c r="R44" s="40">
+        <v>12.794731455542999</v>
+      </c>
+      <c r="S44" s="40">
+        <v>0.99746713955999999</v>
+      </c>
+      <c r="T44" s="40">
+        <v>1.2826068749999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C45" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D45" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E45" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F45" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G45" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H45" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I45" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J45" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K45" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L45" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="M45" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="N45" s="8">
+        <v>5.5379575180000001E-2</v>
+      </c>
+      <c r="O45" s="5">
+        <v>5.1668654783999998E-2</v>
+      </c>
+      <c r="P45" s="5">
+        <v>1.788531748609</v>
+      </c>
+      <c r="Q45" s="5">
+        <v>1.5447759923960001</v>
+      </c>
+      <c r="R45" s="40">
+        <v>4.6269277565899998</v>
+      </c>
+      <c r="S45" s="40">
+        <v>0.54016855772899997</v>
+      </c>
+      <c r="T45" s="40">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="9">
+        <v>0.627</v>
+      </c>
+      <c r="C46" s="11">
+        <v>0</v>
+      </c>
+      <c r="D46" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E46" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F46" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G46" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H46" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I46" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J46" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K46" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L46" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="M46" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="N46" s="8">
+        <v>7.5196853720000002E-3</v>
+      </c>
+      <c r="O46" s="5">
+        <v>7.266812668E-3</v>
+      </c>
+      <c r="P46" s="5">
+        <v>2.1367306718350001</v>
+      </c>
+      <c r="Q46" s="5">
+        <v>1.7789790940529999</v>
+      </c>
+      <c r="R46" s="40">
+        <v>630.45605117503203</v>
+      </c>
+      <c r="S46" s="40">
+        <v>19.721125825418</v>
+      </c>
+      <c r="T46" s="40">
+        <v>24.609375</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="9">
+        <v>0.627</v>
+      </c>
+      <c r="C47" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D47" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E47" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F47" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G47" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H47" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I47" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J47" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K47" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L47" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="M47" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="N47" s="8">
+        <v>3.944565522E-2</v>
+      </c>
+      <c r="O47" s="5">
+        <v>3.7795549754999998E-2</v>
+      </c>
+      <c r="P47" s="5">
+        <v>1.8851469270050001</v>
+      </c>
+      <c r="Q47" s="5">
+        <v>1.6052439952290001</v>
+      </c>
+      <c r="R47" s="40">
+        <v>39.395178165163003</v>
+      </c>
+      <c r="S47" s="40">
+        <v>2.5846971547109998</v>
+      </c>
+      <c r="T47" s="40">
+        <v>3.303589746094</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="9">
+        <v>0.627</v>
+      </c>
+      <c r="C48" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D48" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E48" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F48" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G48" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H48" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I48" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J48" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K48" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L48" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="M48" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="N48" s="8">
+        <v>5.3019316369000001E-2</v>
+      </c>
+      <c r="O48" s="5">
+        <v>5.0644120644E-2</v>
+      </c>
+      <c r="P48" s="5">
+        <v>1.8188438460709999</v>
+      </c>
+      <c r="Q48" s="5">
+        <v>1.564844700416</v>
+      </c>
+      <c r="R48" s="40">
+        <v>11.474521097181</v>
+      </c>
+      <c r="S48" s="40">
+        <v>1.085713514501</v>
+      </c>
+      <c r="T48" s="40">
+        <v>1.375105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C49" s="11">
+        <v>0</v>
+      </c>
+      <c r="D49" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E49" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F49" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G49" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H49" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I49" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J49" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K49" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L49" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="M49" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="N49" s="8">
+        <v>4.584838412E-3</v>
+      </c>
+      <c r="O49" s="5">
+        <v>4.5972564990000003E-3</v>
+      </c>
+      <c r="P49" s="5">
+        <v>2.2518210777140002</v>
+      </c>
+      <c r="Q49" s="5">
+        <v>1.854332485834</v>
+      </c>
+      <c r="R49" s="40">
+        <v>6393.0799960813001</v>
+      </c>
+      <c r="S49" s="40">
+        <v>184.957508404724</v>
+      </c>
+      <c r="T49" s="40">
+        <v>228.125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C50" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D50" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E50" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F50" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G50" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H50" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I50" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J50" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K50" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L50" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="M50" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="N50" s="8">
+        <v>3.3778703894999998E-2</v>
+      </c>
+      <c r="O50" s="5">
+        <v>3.3511987141000003E-2</v>
+      </c>
+      <c r="P50" s="5">
+        <v>1.943117232791</v>
+      </c>
+      <c r="Q50" s="5">
+        <v>1.6444761029920001</v>
+      </c>
+      <c r="R50" s="40">
+        <v>179.75923863906399</v>
+      </c>
+      <c r="S50" s="40">
+        <v>9.9347547579820006</v>
+      </c>
+      <c r="T50" s="40">
+        <v>12.4690671875</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C51" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D51" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E51" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F51" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G51" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H51" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I51" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J51" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K51" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L51" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="M51" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="N51" s="8">
+        <v>4.8940829317000001E-2</v>
+      </c>
+      <c r="O51" s="5">
+        <v>4.8313815325000002E-2</v>
+      </c>
+      <c r="P51" s="5">
+        <v>1.864169846542</v>
+      </c>
+      <c r="Q51" s="5">
+        <v>1.5950985338829999</v>
+      </c>
+      <c r="R51" s="40">
+        <v>38.022146954187001</v>
+      </c>
+      <c r="S51" s="40">
+        <v>2.96462046134</v>
+      </c>
+      <c r="T51" s="40">
+        <v>3.6850000000000001</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
simulate financially constrained firms
simulate financially constrained firms
</commit_message>
<xml_diff>
--- a/model/scenario_stack.xlsx
+++ b/model/scenario_stack.xlsx
@@ -4950,10 +4950,10 @@
   <dimension ref="A1:Y51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N50" sqref="N50"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7476,37 +7476,37 @@
         <v>0.03</v>
       </c>
       <c r="N34" s="8">
-        <v>7.4476376269999997E-3</v>
+        <v>7.3890961710000001E-3</v>
       </c>
       <c r="O34" s="5">
-        <v>7.0167558419999996E-3</v>
+        <v>6.9617070579999999E-3</v>
       </c>
       <c r="P34" s="5">
-        <v>2.6016092097230001</v>
+        <v>2.6015445989699999</v>
       </c>
       <c r="Q34" s="5">
-        <v>1.9143591638220001</v>
+        <v>1.913809067194</v>
       </c>
       <c r="R34" s="68">
-        <v>101.65827248412999</v>
+        <v>101.699215408141</v>
       </c>
       <c r="S34" s="68">
-        <v>3.1680015596220001</v>
+        <v>3.1573596329470002</v>
       </c>
       <c r="T34" s="68">
-        <v>5.1153789062500001</v>
+        <v>5.0674222287559996</v>
       </c>
       <c r="U34" s="10">
-        <v>2.124998272544</v>
+        <v>2.1284911164799998</v>
       </c>
       <c r="V34" s="16">
-        <v>0.38599551944400001</v>
+        <v>0.384692957329</v>
       </c>
       <c r="W34" s="35">
-        <v>0.66105638395199995</v>
+        <v>0.66219819775599997</v>
       </c>
       <c r="X34" s="35">
-        <v>0.86315656003300001</v>
+        <v>0.86448679854099997</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.2">
@@ -7550,37 +7550,37 @@
         <v>0.03</v>
       </c>
       <c r="N35" s="8">
-        <v>3.5916097708E-2</v>
+        <v>3.5637682482999998E-2</v>
       </c>
       <c r="O35" s="5">
-        <v>3.3645512422E-2</v>
+        <v>3.3386797040999998E-2</v>
       </c>
       <c r="P35" s="5">
-        <v>2.3303023956720001</v>
+        <v>2.3266583966060002</v>
       </c>
       <c r="Q35" s="5">
-        <v>1.814562325424</v>
+        <v>1.810885146607</v>
       </c>
       <c r="R35" s="68">
-        <v>12.054047239313</v>
+        <v>12.058820928453001</v>
       </c>
       <c r="S35" s="68">
-        <v>0.81407588392999997</v>
+        <v>0.80665011879799997</v>
       </c>
       <c r="T35" s="68">
-        <v>1.234509117187</v>
+        <v>1.203646389075</v>
       </c>
       <c r="U35" s="10">
-        <v>3.7064201659939999</v>
+        <v>3.7320225332870001</v>
       </c>
       <c r="V35" s="16">
-        <v>0.30725068092399999</v>
+        <v>0.30381714903599999</v>
       </c>
       <c r="W35" s="35">
-        <v>0.47764834014699997</v>
+        <v>0.47990762164700002</v>
       </c>
       <c r="X35" s="35">
-        <v>0.62040628076600002</v>
+        <v>0.62255663553899998</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.2">
@@ -7624,37 +7624,37 @@
         <v>0.03</v>
       </c>
       <c r="N36" s="8">
-        <v>4.7847410554999997E-2</v>
+        <v>4.7972467957999997E-2</v>
       </c>
       <c r="O36" s="5">
-        <v>4.4735301406000003E-2</v>
+        <v>4.4850887919999999E-2</v>
       </c>
       <c r="P36" s="5">
-        <v>2.250594920608</v>
+        <v>2.250652263389</v>
       </c>
       <c r="Q36" s="5">
-        <v>1.7848379986759999</v>
+        <v>1.7857123390230001</v>
       </c>
       <c r="R36" s="68">
-        <v>4.4860160390130002</v>
+        <v>4.4850608847059998</v>
       </c>
       <c r="S36" s="68">
-        <v>0.44395988984899998</v>
+        <v>0.44566993641399999</v>
       </c>
       <c r="T36" s="68">
-        <v>0.64687499999999998</v>
+        <v>0.65496093749999995</v>
       </c>
       <c r="U36" s="10">
-        <v>5.1451031890800003</v>
+        <v>5.1240707945050001</v>
       </c>
       <c r="V36" s="16">
-        <v>0.27255785539400001</v>
+        <v>0.27416447633500002</v>
       </c>
       <c r="W36" s="35">
-        <v>0.38913058205899997</v>
+        <v>0.38830815155999998</v>
       </c>
       <c r="X36" s="35">
-        <v>0.50234652331700003</v>
+        <v>0.50172450275199998</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.2">
@@ -7698,37 +7698,37 @@
         <v>0.03</v>
       </c>
       <c r="N37" s="8">
-        <v>4.8958288310000002E-3</v>
+        <v>4.9328477629999997E-3</v>
       </c>
       <c r="O37" s="5">
-        <v>4.7343536409999998E-3</v>
+        <v>4.7701002950000003E-3</v>
       </c>
       <c r="P37" s="5">
-        <v>2.718477314717</v>
+        <v>2.7200482714629999</v>
       </c>
       <c r="Q37" s="5">
-        <v>1.939954736851</v>
+        <v>1.941020286973</v>
       </c>
       <c r="R37" s="68">
-        <v>514.01780708035005</v>
+        <v>513.86973280632299</v>
       </c>
       <c r="S37" s="68">
-        <v>14.769511428245</v>
+        <v>14.808637434623</v>
       </c>
       <c r="T37" s="68">
-        <v>24.3017578125</v>
+        <v>24.358715054867002</v>
       </c>
       <c r="U37" s="10">
-        <v>1.8381332181500001</v>
+        <v>1.8386034632970001</v>
       </c>
       <c r="V37" s="16">
-        <v>0.43414786677</v>
+        <v>0.43464075135000002</v>
       </c>
       <c r="W37" s="35">
-        <v>0.67908894578800005</v>
+        <v>0.67814214752699997</v>
       </c>
       <c r="X37" s="35">
-        <v>0.88713159633600003</v>
+        <v>0.88589416349200001</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.2">
@@ -7772,37 +7772,37 @@
         <v>0.03</v>
       </c>
       <c r="N38" s="8">
-        <v>3.2464685788999997E-2</v>
+        <v>3.2197502854999997E-2</v>
       </c>
       <c r="O38" s="5">
-        <v>3.1176542192999999E-2</v>
+        <v>3.0922383768000002E-2</v>
       </c>
       <c r="P38" s="5">
-        <v>2.3986427744799999</v>
+        <v>2.3957885727920001</v>
       </c>
       <c r="Q38" s="5">
-        <v>1.8362379888360001</v>
+        <v>1.8341235743199999</v>
       </c>
       <c r="R38" s="68">
-        <v>36.494268926906003</v>
+        <v>36.514120132404003</v>
       </c>
       <c r="S38" s="68">
-        <v>2.1108616673860001</v>
+        <v>2.0923396021910001</v>
       </c>
       <c r="T38" s="68">
-        <v>3.1797051305249999</v>
+        <v>3.1393377807039999</v>
       </c>
       <c r="U38" s="10">
-        <v>3.018892337479</v>
+        <v>3.0223645800660002</v>
       </c>
       <c r="V38" s="16">
-        <v>0.34743688415099999</v>
+        <v>0.34546851162699999</v>
       </c>
       <c r="W38" s="35">
-        <v>0.51826676757099999</v>
+        <v>0.52065539873699995</v>
       </c>
       <c r="X38" s="35">
-        <v>0.67334823552400003</v>
+        <v>0.67628598570099996</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.2">
@@ -7846,37 +7846,37 @@
         <v>0.03</v>
       </c>
       <c r="N39" s="8">
-        <v>4.5924088449999997E-2</v>
+        <v>4.5753599609000002E-2</v>
       </c>
       <c r="O39" s="5">
-        <v>4.3975270694999999E-2</v>
+        <v>4.3814211659999998E-2</v>
       </c>
       <c r="P39" s="5">
-        <v>2.3029563059639999</v>
+        <v>2.2989321404590002</v>
       </c>
       <c r="Q39" s="5">
-        <v>1.8029988650740001</v>
+        <v>1.801042356807</v>
       </c>
       <c r="R39" s="68">
-        <v>10.978029455899</v>
+        <v>10.983961607873001</v>
       </c>
       <c r="S39" s="68">
-        <v>0.90687738561999998</v>
+        <v>0.90216369038199995</v>
       </c>
       <c r="T39" s="68">
-        <v>1.3235385625</v>
+        <v>1.3170759723600001</v>
       </c>
       <c r="U39" s="10">
-        <v>4.0396487867640003</v>
+        <v>4.0371489632369997</v>
       </c>
       <c r="V39" s="16">
-        <v>0.309507904306</v>
+        <v>0.30870345892899997</v>
       </c>
       <c r="W39" s="35">
-        <v>0.43602257975399999</v>
+        <v>0.437417046985</v>
       </c>
       <c r="X39" s="35">
-        <v>0.56365251445700004</v>
+        <v>0.56548651864800004</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.2">
@@ -7920,37 +7920,37 @@
         <v>0.03</v>
       </c>
       <c r="N40" s="8">
-        <v>2.8310513069999999E-3</v>
+        <v>2.8175569740000002E-3</v>
       </c>
       <c r="O40" s="5">
-        <v>2.8401282489999998E-3</v>
+        <v>2.8266037849999999E-3</v>
       </c>
       <c r="P40" s="5">
-        <v>2.8749879887250001</v>
+        <v>2.8735446417819999</v>
       </c>
       <c r="Q40" s="5">
-        <v>1.9732370109290001</v>
+        <v>1.9722087181700001</v>
       </c>
       <c r="R40" s="68">
-        <v>4915.7362497793001</v>
+        <v>4916.6786699054301</v>
       </c>
       <c r="S40" s="68">
-        <v>133.10279839031699</v>
+        <v>132.92945143268801</v>
       </c>
       <c r="T40" s="68">
-        <v>225.2734375</v>
+        <v>225.40543365478501</v>
       </c>
       <c r="U40" s="10">
-        <v>1.6255885311130001</v>
+        <v>1.6247578148399999</v>
       </c>
       <c r="V40" s="16">
-        <v>0.48419461496900001</v>
+        <v>0.48408474680199998</v>
       </c>
       <c r="W40" s="35">
-        <v>0.68815316768900003</v>
+        <v>0.68866379871100003</v>
       </c>
       <c r="X40" s="35">
-        <v>0.89945039020700002</v>
+        <v>0.90014898161500001</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.2">
@@ -7994,37 +7994,37 @@
         <v>0.03</v>
       </c>
       <c r="N41" s="8">
-        <v>2.7159211086000001E-2</v>
+        <v>2.7243058779E-2</v>
       </c>
       <c r="O41" s="5">
-        <v>2.7020122717000002E-2</v>
+        <v>2.7102555702999999E-2</v>
       </c>
       <c r="P41" s="5">
-        <v>2.4885233679269998</v>
+        <v>2.490143377011</v>
       </c>
       <c r="Q41" s="5">
-        <v>1.8641023722359999</v>
+        <v>1.8649202338069999</v>
       </c>
       <c r="R41" s="68">
-        <v>162.443631113414</v>
+        <v>162.42864808014099</v>
       </c>
       <c r="S41" s="68">
-        <v>8.0434752451320009</v>
+        <v>8.0666463323070001</v>
       </c>
       <c r="T41" s="68">
-        <v>12.15734051025</v>
+        <v>12.309307266375001</v>
       </c>
       <c r="U41" s="10">
-        <v>2.5021469287250002</v>
+        <v>2.4936601678480002</v>
       </c>
       <c r="V41" s="16">
-        <v>0.390106072222</v>
+        <v>0.39186810973500003</v>
       </c>
       <c r="W41" s="35">
-        <v>0.556407154791</v>
+        <v>0.55569105681800002</v>
       </c>
       <c r="X41" s="35">
-        <v>0.72367470210100004</v>
+        <v>0.72315880768100005</v>
       </c>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
@@ -8068,37 +8068,37 @@
         <v>0.03</v>
       </c>
       <c r="N42" s="8">
-        <v>4.1408603815E-2</v>
+        <v>4.1814717132000002E-2</v>
       </c>
       <c r="O42" s="5">
-        <v>4.1017908149999997E-2</v>
+        <v>4.1413592397000001E-2</v>
       </c>
       <c r="P42" s="5">
-        <v>2.3742803384540001</v>
+        <v>2.3772578897379999</v>
       </c>
       <c r="Q42" s="5">
-        <v>1.8289507105909999</v>
+        <v>1.831500762611</v>
       </c>
       <c r="R42" s="68">
-        <v>35.773568502126999</v>
+        <v>35.753100829746998</v>
       </c>
       <c r="S42" s="68">
-        <v>2.4433747943639998</v>
+        <v>2.4733025538760001</v>
       </c>
       <c r="T42" s="68">
-        <v>3.56984375</v>
+        <v>3.6590898437499999</v>
       </c>
       <c r="U42" s="10">
-        <v>3.2343107635089998</v>
+        <v>3.2187576969810001</v>
       </c>
       <c r="V42" s="16">
-        <v>0.34794866681600001</v>
+        <v>0.351697841751</v>
       </c>
       <c r="W42" s="35">
-        <v>0.48389393189399998</v>
+        <v>0.48087345153599997</v>
       </c>
       <c r="X42" s="35">
-        <v>0.62648333068399997</v>
+        <v>0.623181295977</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.2">
@@ -8142,37 +8142,37 @@
         <v>0.05</v>
       </c>
       <c r="N43" s="8">
-        <v>5.4556652779999999E-3</v>
+        <v>5.3859023610000004E-3</v>
       </c>
       <c r="O43" s="5">
-        <v>5.1423019570000002E-3</v>
+        <v>5.076642349E-3</v>
       </c>
       <c r="P43" s="5">
-        <v>2.8170224232769998</v>
+        <v>2.8165990491790001</v>
       </c>
       <c r="Q43" s="5">
-        <v>1.975049363696</v>
+        <v>1.9742936897159999</v>
       </c>
       <c r="R43" s="68">
-        <v>89.810064923162003</v>
+        <v>89.950986081406995</v>
       </c>
       <c r="S43" s="68">
-        <v>2.5697787241559999</v>
+        <v>2.557027428269</v>
       </c>
       <c r="T43" s="68">
-        <v>4.6918125000000002</v>
+        <v>4.6624886718749998</v>
       </c>
       <c r="U43" s="10">
-        <v>2.1473745001490001</v>
+        <v>2.1462201203419999</v>
       </c>
       <c r="V43" s="16">
-        <v>0.36943778722699999</v>
+        <v>0.36845872756600001</v>
       </c>
       <c r="W43" s="35">
-        <v>0.68446501347800004</v>
+        <v>0.68665685994299996</v>
       </c>
       <c r="X43" s="35">
-        <v>0.89671359409600004</v>
+        <v>0.89950988068000004</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.2">
@@ -8216,37 +8216,37 @@
         <v>0.05</v>
       </c>
       <c r="N44" s="8">
-        <v>3.0590178297999999E-2</v>
+        <v>3.0396316626000001E-2</v>
       </c>
       <c r="O44" s="5">
-        <v>2.8689823558999999E-2</v>
+        <v>2.8509465267999998E-2</v>
       </c>
       <c r="P44" s="5">
-        <v>2.5367629341410001</v>
+        <v>2.5353751963039999</v>
       </c>
       <c r="Q44" s="5">
-        <v>1.9058732348930001</v>
+        <v>1.9053130278929999</v>
       </c>
       <c r="R44" s="68">
-        <v>11.361170545394</v>
+        <v>11.379634341960999</v>
       </c>
       <c r="S44" s="68">
-        <v>0.67686538542499997</v>
+        <v>0.67122405056699996</v>
       </c>
       <c r="T44" s="68">
-        <v>1.122281015625</v>
+        <v>1.094223983911</v>
       </c>
       <c r="U44" s="10">
-        <v>3.6645142342970001</v>
+        <v>3.6867232972220001</v>
       </c>
       <c r="V44" s="16">
-        <v>0.29330198520400003</v>
+        <v>0.29007437544999998</v>
       </c>
       <c r="W44" s="35">
-        <v>0.50524374230900004</v>
+        <v>0.50783092639299998</v>
       </c>
       <c r="X44" s="35">
-        <v>0.66136020666600004</v>
+        <v>0.66387242742700003</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.2">
@@ -8290,37 +8290,37 @@
         <v>0.05</v>
       </c>
       <c r="N45" s="8">
-        <v>4.2005677812999999E-2</v>
+        <v>4.1884958894999998E-2</v>
       </c>
       <c r="O45" s="5">
-        <v>3.9324130305000003E-2</v>
+        <v>3.9212531597E-2</v>
       </c>
       <c r="P45" s="5">
-        <v>2.4434320049860001</v>
+        <v>2.4419676921089999</v>
       </c>
       <c r="Q45" s="5">
-        <v>1.882100874432</v>
+        <v>1.8811493437569999</v>
       </c>
       <c r="R45" s="68">
-        <v>4.3041820767010002</v>
+        <v>4.3129056728539998</v>
       </c>
       <c r="S45" s="68">
-        <v>0.37122572957299999</v>
+        <v>0.36912582408799999</v>
       </c>
       <c r="T45" s="68">
-        <v>0.58650000000000002</v>
+        <v>0.58271982421900004</v>
       </c>
       <c r="U45" s="10">
-        <v>5.0377004668160001</v>
+        <v>5.0310028176569999</v>
       </c>
       <c r="V45" s="16">
-        <v>0.25894599617500003</v>
+        <v>0.25808238063400002</v>
       </c>
       <c r="W45" s="35">
-        <v>0.41687080741100002</v>
+        <v>0.41883051948900002</v>
       </c>
       <c r="X45" s="35">
-        <v>0.54342032704099996</v>
+        <v>0.54592907123800005</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.2">
@@ -8364,37 +8364,37 @@
         <v>0.05</v>
       </c>
       <c r="N46" s="8">
-        <v>3.5059767230000002E-3</v>
+        <v>3.508901238E-3</v>
       </c>
       <c r="O46" s="5">
-        <v>3.3915068960000002E-3</v>
+        <v>3.3943331079999998E-3</v>
       </c>
       <c r="P46" s="5">
-        <v>2.9475415985370002</v>
+        <v>2.9476790312559999</v>
       </c>
       <c r="Q46" s="5">
-        <v>1.9865454114309999</v>
+        <v>1.986528250244</v>
       </c>
       <c r="R46" s="68">
-        <v>441.89720650633302</v>
+        <v>441.90020693285999</v>
       </c>
       <c r="S46" s="68">
-        <v>11.854393736732</v>
+        <v>11.858146345844</v>
       </c>
       <c r="T46" s="68">
-        <v>22.60986328125</v>
+        <v>22.623111246766001</v>
       </c>
       <c r="U46" s="10">
-        <v>1.859024206617</v>
+        <v>1.858905884049</v>
       </c>
       <c r="V46" s="16">
-        <v>0.41817127735999998</v>
+        <v>0.41826122403400001</v>
       </c>
       <c r="W46" s="35">
-        <v>0.69809078721399997</v>
+        <v>0.697986161833</v>
       </c>
       <c r="X46" s="35">
-        <v>0.91497932558399997</v>
+        <v>0.91485060835900001</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
@@ -8438,37 +8438,37 @@
         <v>0.05</v>
       </c>
       <c r="N47" s="8">
-        <v>2.7281682599999999E-2</v>
+        <v>2.7319876855000001E-2</v>
       </c>
       <c r="O47" s="5">
-        <v>2.6236500833000002E-2</v>
+        <v>2.6272990821999999E-2</v>
       </c>
       <c r="P47" s="5">
-        <v>2.616606589106</v>
+        <v>2.6182657818599999</v>
       </c>
       <c r="Q47" s="5">
-        <v>1.9244265920950001</v>
+        <v>1.9263368002229999</v>
       </c>
       <c r="R47" s="68">
-        <v>34.017685350839002</v>
+        <v>34.028458764753999</v>
       </c>
       <c r="S47" s="68">
-        <v>1.7515318219539999</v>
+        <v>1.75424347529</v>
       </c>
       <c r="T47" s="68">
-        <v>2.931935899575</v>
+        <v>2.9141839443549999</v>
       </c>
       <c r="U47" s="10">
-        <v>2.981832258611</v>
+        <v>2.9902422627190002</v>
       </c>
       <c r="V47" s="16">
-        <v>0.33434569932699998</v>
+        <v>0.33364927362800001</v>
       </c>
       <c r="W47" s="35">
-        <v>0.54428881989699995</v>
+        <v>0.54390210430099994</v>
       </c>
       <c r="X47" s="35">
-        <v>0.71275808809899999</v>
+        <v>0.71189369453999995</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.2">
@@ -8512,37 +8512,37 @@
         <v>0.05</v>
       </c>
       <c r="N48" s="8">
-        <v>3.9833791961000002E-2</v>
+        <v>4.0071067342999998E-2</v>
       </c>
       <c r="O48" s="5">
-        <v>3.8208055381E-2</v>
+        <v>3.8433482398999998E-2</v>
       </c>
       <c r="P48" s="5">
-        <v>2.508335909495</v>
+        <v>2.5127986323860001</v>
       </c>
       <c r="Q48" s="5">
-        <v>1.900036213128</v>
+        <v>1.901276080785</v>
       </c>
       <c r="R48" s="68">
-        <v>10.463243351591</v>
+        <v>10.466873692492999</v>
       </c>
       <c r="S48" s="68">
-        <v>0.753668268631</v>
+        <v>0.76016330623700001</v>
       </c>
       <c r="T48" s="68">
-        <v>1.2032168750000001</v>
+        <v>1.210736980469</v>
       </c>
       <c r="U48" s="10">
-        <v>3.955047613124</v>
+        <v>3.9587947162030002</v>
       </c>
       <c r="V48" s="16">
-        <v>0.29542766444399998</v>
+        <v>0.29646678164200002</v>
       </c>
       <c r="W48" s="35">
-        <v>0.46502354310100003</v>
+        <v>0.462968039981</v>
       </c>
       <c r="X48" s="35">
-        <v>0.60692656348100005</v>
+        <v>0.60412399437999997</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.2">
@@ -8586,37 +8586,37 @@
         <v>0.05</v>
       </c>
       <c r="N49" s="8">
-        <v>1.9165202119999999E-3</v>
+        <v>1.916153124E-3</v>
       </c>
       <c r="O49" s="5">
-        <v>1.923157867E-3</v>
+        <v>1.922789668E-3</v>
       </c>
       <c r="P49" s="5">
-        <v>3.10467028399</v>
+        <v>3.104447332791</v>
       </c>
       <c r="Q49" s="5">
-        <v>1.9909264166930001</v>
+        <v>1.990770069114</v>
       </c>
       <c r="R49" s="68">
-        <v>4064.1618000743601</v>
+        <v>4063.9004758534102</v>
       </c>
       <c r="S49" s="68">
-        <v>103.616318520603</v>
+        <v>103.605693752908</v>
       </c>
       <c r="T49" s="68">
-        <v>209.58984375</v>
+        <v>209.54890828363301</v>
       </c>
       <c r="U49" s="10">
-        <v>1.6480168615349999</v>
+        <v>1.648085053877</v>
       </c>
       <c r="V49" s="16">
-        <v>0.46671110934400001</v>
+        <v>0.46668341023400001</v>
       </c>
       <c r="W49" s="35">
-        <v>0.70516902848899998</v>
+        <v>0.70518159165299998</v>
       </c>
       <c r="X49" s="35">
-        <v>0.92468992255899995</v>
+        <v>0.92470402135999996</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.2">
@@ -8660,37 +8660,37 @@
         <v>0.05</v>
       </c>
       <c r="N50" s="8">
-        <v>2.2531751799000001E-2</v>
+        <v>2.2616050897000001E-2</v>
       </c>
       <c r="O50" s="5">
-        <v>2.2454848413000002E-2</v>
+        <v>2.2538056808000001E-2</v>
       </c>
       <c r="P50" s="5">
-        <v>2.7229728558650002</v>
+        <v>2.7240910689070001</v>
       </c>
       <c r="Q50" s="5">
-        <v>1.947712053192</v>
+        <v>1.9485570637159999</v>
       </c>
       <c r="R50" s="68">
-        <v>148.99230557019601</v>
+        <v>148.95090733415</v>
       </c>
       <c r="S50" s="68">
-        <v>6.6821733245989998</v>
+        <v>6.7070100998570004</v>
       </c>
       <c r="T50" s="68">
-        <v>11.378023810875</v>
+        <v>11.37802381</v>
       </c>
       <c r="U50" s="10">
-        <v>2.4790868066509999</v>
+        <v>2.4828945102510001</v>
       </c>
       <c r="V50" s="16">
-        <v>0.378158642037</v>
+        <v>0.37833181377000002</v>
       </c>
       <c r="W50" s="35">
-        <v>0.57837096649599995</v>
+        <v>0.57721824766200003</v>
       </c>
       <c r="X50" s="35">
-        <v>0.75788972704699997</v>
+        <v>0.75623262736600005</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.2">
@@ -8734,37 +8734,37 @@
         <v>0.05</v>
       </c>
       <c r="N51" s="8">
-        <v>3.6041646704999999E-2</v>
+        <v>3.5857065969999997E-2</v>
       </c>
       <c r="O51" s="5">
-        <v>3.5773826016000002E-2</v>
+        <v>3.5593186994999998E-2</v>
       </c>
       <c r="P51" s="5">
-        <v>2.6001683298659999</v>
+        <v>2.5966152982409998</v>
       </c>
       <c r="Q51" s="5">
-        <v>1.926821638399</v>
+        <v>1.923989066828</v>
       </c>
       <c r="R51" s="68">
-        <v>33.676961842658002</v>
+        <v>33.689782715881002</v>
       </c>
       <c r="S51" s="68">
-        <v>2.0723514145639998</v>
+        <v>2.057957182425</v>
       </c>
       <c r="T51" s="68">
-        <v>3.3165</v>
+        <v>3.298362890625</v>
       </c>
       <c r="U51" s="10">
-        <v>3.1899980061569999</v>
+        <v>3.186816635449</v>
       </c>
       <c r="V51" s="16">
-        <v>0.336738578407</v>
+        <v>0.33577339530900002</v>
       </c>
       <c r="W51" s="35">
-        <v>0.50544121888399995</v>
+        <v>0.507393625811</v>
       </c>
       <c r="X51" s="35">
-        <v>0.65993273123200002</v>
+        <v>0.662550642488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add one more scenario: less-constrained firms
add one more scenario: less-constrained firms
</commit_message>
<xml_diff>
--- a/model/scenario_stack.xlsx
+++ b/model/scenario_stack.xlsx
@@ -1173,7 +1173,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1375,6 +1375,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4947,13 +4950,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y51"/>
+  <dimension ref="A1:Y60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="S52" sqref="S52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8767,6 +8770,564 @@
         <v>0.662550642488</v>
       </c>
     </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C52" s="11">
+        <v>0</v>
+      </c>
+      <c r="D52" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E52" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F52" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G52" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H52" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I52" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J52" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K52" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L52" s="69">
+        <v>0.01</v>
+      </c>
+      <c r="M52" s="69">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N52" s="8">
+        <v>7.3890961710000001E-3</v>
+      </c>
+      <c r="O52" s="5">
+        <v>6.9617070579999999E-3</v>
+      </c>
+      <c r="P52" s="5">
+        <v>2.6015445989699999</v>
+      </c>
+      <c r="Q52" s="5">
+        <v>1.913809067194</v>
+      </c>
+      <c r="R52" s="68">
+        <v>101.699215408141</v>
+      </c>
+      <c r="S52" s="68">
+        <v>3.1573596329470002</v>
+      </c>
+      <c r="T52" s="68">
+        <v>5.0674222287559996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C53" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D53" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E53" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F53" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G53" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H53" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I53" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J53" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K53" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L53" s="69">
+        <v>0.01</v>
+      </c>
+      <c r="M53" s="69">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N53" s="8">
+        <v>3.5637682482999998E-2</v>
+      </c>
+      <c r="O53" s="5">
+        <v>3.3386797040999998E-2</v>
+      </c>
+      <c r="P53" s="5">
+        <v>2.3266583966060002</v>
+      </c>
+      <c r="Q53" s="5">
+        <v>1.810885146607</v>
+      </c>
+      <c r="R53" s="68">
+        <v>12.058820928453001</v>
+      </c>
+      <c r="S53" s="68">
+        <v>0.80665011879799997</v>
+      </c>
+      <c r="T53" s="68">
+        <v>1.203646389075</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C54" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D54" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E54" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F54" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G54" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H54" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I54" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J54" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K54" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L54" s="69">
+        <v>0.01</v>
+      </c>
+      <c r="M54" s="69">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N54" s="8">
+        <v>4.7972467957999997E-2</v>
+      </c>
+      <c r="O54" s="5">
+        <v>4.4850887919999999E-2</v>
+      </c>
+      <c r="P54" s="5">
+        <v>2.250652263389</v>
+      </c>
+      <c r="Q54" s="5">
+        <v>1.7857123390230001</v>
+      </c>
+      <c r="R54" s="68">
+        <v>4.4850608847059998</v>
+      </c>
+      <c r="S54" s="68">
+        <v>0.44566993641399999</v>
+      </c>
+      <c r="T54" s="68">
+        <v>0.65496093749999995</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="9">
+        <v>0.627</v>
+      </c>
+      <c r="C55" s="11">
+        <v>0</v>
+      </c>
+      <c r="D55" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E55" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F55" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G55" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H55" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I55" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J55" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K55" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L55" s="69">
+        <v>0.01</v>
+      </c>
+      <c r="M55" s="69">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N55" s="8">
+        <v>4.9328477629999997E-3</v>
+      </c>
+      <c r="O55" s="5">
+        <v>4.7701002950000003E-3</v>
+      </c>
+      <c r="P55" s="5">
+        <v>2.7200482714629999</v>
+      </c>
+      <c r="Q55" s="5">
+        <v>1.941020286973</v>
+      </c>
+      <c r="R55" s="68">
+        <v>513.86973280632299</v>
+      </c>
+      <c r="S55" s="68">
+        <v>14.808637434623</v>
+      </c>
+      <c r="T55" s="68">
+        <v>24.358715054867002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="9">
+        <v>0.627</v>
+      </c>
+      <c r="C56" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D56" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E56" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F56" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G56" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H56" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I56" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J56" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K56" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L56" s="69">
+        <v>0.01</v>
+      </c>
+      <c r="M56" s="69">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N56" s="8">
+        <v>3.2197502854999997E-2</v>
+      </c>
+      <c r="O56" s="5">
+        <v>3.0922383768000002E-2</v>
+      </c>
+      <c r="P56" s="5">
+        <v>2.3957885727920001</v>
+      </c>
+      <c r="Q56" s="5">
+        <v>1.8341235743199999</v>
+      </c>
+      <c r="R56" s="68">
+        <v>36.514120132404003</v>
+      </c>
+      <c r="S56" s="68">
+        <v>2.0923396021910001</v>
+      </c>
+      <c r="T56" s="68">
+        <v>3.1393377807039999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="9">
+        <v>0.627</v>
+      </c>
+      <c r="C57" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D57" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E57" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F57" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G57" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H57" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I57" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J57" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K57" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L57" s="69">
+        <v>0.01</v>
+      </c>
+      <c r="M57" s="69">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N57" s="8">
+        <v>4.5753599609000002E-2</v>
+      </c>
+      <c r="O57" s="5">
+        <v>4.3814211659999998E-2</v>
+      </c>
+      <c r="P57" s="5">
+        <v>2.2989321404590002</v>
+      </c>
+      <c r="Q57" s="5">
+        <v>1.801042356807</v>
+      </c>
+      <c r="R57" s="68">
+        <v>10.983961607873001</v>
+      </c>
+      <c r="S57" s="68">
+        <v>0.90216369038199995</v>
+      </c>
+      <c r="T57" s="68">
+        <v>1.3170759723600001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C58" s="11">
+        <v>0</v>
+      </c>
+      <c r="D58" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E58" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F58" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G58" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H58" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I58" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J58" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K58" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L58" s="69">
+        <v>0.01</v>
+      </c>
+      <c r="M58" s="69">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N58" s="8">
+        <v>2.8175569740000002E-3</v>
+      </c>
+      <c r="O58" s="5">
+        <v>2.8266037849999999E-3</v>
+      </c>
+      <c r="P58" s="5">
+        <v>2.8735446417819999</v>
+      </c>
+      <c r="Q58" s="5">
+        <v>1.9722087181700001</v>
+      </c>
+      <c r="R58" s="68">
+        <v>4916.6786699054301</v>
+      </c>
+      <c r="S58" s="68">
+        <v>132.92945143268801</v>
+      </c>
+      <c r="T58" s="68">
+        <v>225.40543365478501</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C59" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D59" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E59" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F59" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G59" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H59" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I59" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J59" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K59" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L59" s="69">
+        <v>0.01</v>
+      </c>
+      <c r="M59" s="69">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N59" s="8">
+        <v>2.7243058779E-2</v>
+      </c>
+      <c r="O59" s="5">
+        <v>2.7102555702999999E-2</v>
+      </c>
+      <c r="P59" s="5">
+        <v>2.490143377011</v>
+      </c>
+      <c r="Q59" s="5">
+        <v>1.8649202338069999</v>
+      </c>
+      <c r="R59" s="68">
+        <v>162.42864808014099</v>
+      </c>
+      <c r="S59" s="68">
+        <v>8.0666463323070001</v>
+      </c>
+      <c r="T59" s="68">
+        <v>12.309307266375001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="C60" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D60" s="14">
+        <v>-0.18</v>
+      </c>
+      <c r="E60" s="14">
+        <v>0.06</v>
+      </c>
+      <c r="F60" s="14">
+        <v>0.34</v>
+      </c>
+      <c r="G60" s="14">
+        <v>0.19</v>
+      </c>
+      <c r="H60" s="14">
+        <v>0.45</v>
+      </c>
+      <c r="I60" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="J60" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K60" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="L60" s="69">
+        <v>0.01</v>
+      </c>
+      <c r="M60" s="69">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N60" s="8">
+        <v>4.1814717132000002E-2</v>
+      </c>
+      <c r="O60" s="5">
+        <v>4.1413592397000001E-2</v>
+      </c>
+      <c r="P60" s="5">
+        <v>2.3772578897379999</v>
+      </c>
+      <c r="Q60" s="5">
+        <v>1.831500762611</v>
+      </c>
+      <c r="R60" s="68">
+        <v>35.753100829746998</v>
+      </c>
+      <c r="S60" s="68">
+        <v>2.4733025538760001</v>
+      </c>
+      <c r="T60" s="68">
+        <v>3.6590898437499999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
add the optimization results of less-constrained firms
add the optimization results of less-constrained firms
</commit_message>
<xml_diff>
--- a/model/scenario_stack.xlsx
+++ b/model/scenario_stack.xlsx
@@ -4953,10 +4953,10 @@
   <dimension ref="A1:Y60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S52" sqref="S52"/>
+      <selection pane="bottomRight" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8811,25 +8811,37 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N52" s="8">
-        <v>7.3890961710000001E-3</v>
+        <v>1.1675815967E-2</v>
       </c>
       <c r="O52" s="5">
-        <v>6.9617070579999999E-3</v>
+        <v>1.0988030018E-2</v>
       </c>
       <c r="P52" s="5">
-        <v>2.6015445989699999</v>
+        <v>1.693066138998</v>
       </c>
       <c r="Q52" s="5">
-        <v>1.913809067194</v>
+        <v>1.5309694499449999</v>
       </c>
       <c r="R52" s="68">
-        <v>101.699215408141</v>
+        <v>120.811907979879</v>
       </c>
       <c r="S52" s="68">
-        <v>3.1573596329470002</v>
+        <v>4.2763646614770003</v>
       </c>
       <c r="T52" s="68">
-        <v>5.0674222287559996</v>
+        <v>5.0515865345339996</v>
+      </c>
+      <c r="U52" s="10">
+        <v>2.229535800286</v>
+      </c>
+      <c r="V52" s="16">
+        <v>0.38668183671599998</v>
+      </c>
+      <c r="W52" s="35">
+        <v>0.63268452493899996</v>
+      </c>
+      <c r="X52" s="35">
+        <v>0.81665925758699998</v>
       </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.2">
@@ -8873,25 +8885,37 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N53" s="8">
-        <v>3.5637682482999998E-2</v>
+        <v>4.3941017777999997E-2</v>
       </c>
       <c r="O53" s="5">
-        <v>3.3386797040999998E-2</v>
+        <v>4.1054243781999997E-2</v>
       </c>
       <c r="P53" s="5">
-        <v>2.3266583966060002</v>
+        <v>1.546434727062</v>
       </c>
       <c r="Q53" s="5">
-        <v>1.810885146607</v>
+        <v>1.399208154439</v>
       </c>
       <c r="R53" s="68">
-        <v>12.058820928453001</v>
+        <v>12.528886566156</v>
       </c>
       <c r="S53" s="68">
-        <v>0.80665011879799997</v>
+        <v>1.0223204031390001</v>
       </c>
       <c r="T53" s="68">
-        <v>1.203646389075</v>
+        <v>1.264416426413</v>
+      </c>
+      <c r="U53" s="10">
+        <v>4.0942748305540002</v>
+      </c>
+      <c r="V53" s="16">
+        <v>0.30398230445899999</v>
+      </c>
+      <c r="W53" s="35">
+        <v>0.442374368465</v>
+      </c>
+      <c r="X53" s="35">
+        <v>0.56247309236900001</v>
       </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.2">
@@ -8935,25 +8959,37 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N54" s="8">
-        <v>4.7972467957999997E-2</v>
+        <v>5.5791661999999999E-2</v>
       </c>
       <c r="O54" s="5">
-        <v>4.4850887919999999E-2</v>
+        <v>5.2010193203000002E-2</v>
       </c>
       <c r="P54" s="5">
-        <v>2.250652263389</v>
+        <v>1.513096033591</v>
       </c>
       <c r="Q54" s="5">
-        <v>1.7857123390230001</v>
+        <v>1.3737313002260001</v>
       </c>
       <c r="R54" s="68">
-        <v>4.4850608847059998</v>
+        <v>4.4937827015109999</v>
       </c>
       <c r="S54" s="68">
-        <v>0.44566993641399999</v>
+        <v>0.55174393691300005</v>
       </c>
       <c r="T54" s="68">
-        <v>0.65496093749999995</v>
+        <v>0.68463885550299997</v>
+      </c>
+      <c r="U54" s="10">
+        <v>5.7605952186779996</v>
+      </c>
+      <c r="V54" s="16">
+        <v>0.27309294396900002</v>
+      </c>
+      <c r="W54" s="35">
+        <v>0.351765876496</v>
+      </c>
+      <c r="X54" s="35">
+        <v>0.44372465680399997</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.2">
@@ -8997,25 +9033,37 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N55" s="8">
-        <v>4.9328477629999997E-3</v>
+        <v>8.1897672119999997E-3</v>
       </c>
       <c r="O55" s="5">
-        <v>4.7701002950000003E-3</v>
+        <v>7.91205377E-3</v>
       </c>
       <c r="P55" s="5">
-        <v>2.7200482714629999</v>
+        <v>1.7514860972270001</v>
       </c>
       <c r="Q55" s="5">
-        <v>1.941020286973</v>
+        <v>1.585021037338</v>
       </c>
       <c r="R55" s="68">
-        <v>513.86973280632299</v>
+        <v>644.29736053513295</v>
       </c>
       <c r="S55" s="68">
-        <v>14.808637434623</v>
+        <v>20.647616166904001</v>
       </c>
       <c r="T55" s="68">
-        <v>24.358715054867002</v>
+        <v>23.825868158281001</v>
+      </c>
+      <c r="U55" s="10">
+        <v>1.906389575583</v>
+      </c>
+      <c r="V55" s="16">
+        <v>0.43656936243700001</v>
+      </c>
+      <c r="W55" s="35">
+        <v>0.65482685345299996</v>
+      </c>
+      <c r="X55" s="35">
+        <v>0.84637348485899999</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.2">
@@ -9059,25 +9107,37 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N56" s="8">
-        <v>3.2197502854999997E-2</v>
+        <v>4.0212931409000001E-2</v>
       </c>
       <c r="O56" s="5">
-        <v>3.0922383768000002E-2</v>
+        <v>3.8497365759999999E-2</v>
       </c>
       <c r="P56" s="5">
-        <v>2.3957885727920001</v>
+        <v>1.5768812956239999</v>
       </c>
       <c r="Q56" s="5">
-        <v>1.8341235743199999</v>
+        <v>1.425203107018</v>
       </c>
       <c r="R56" s="68">
-        <v>36.514120132404003</v>
+        <v>38.828523486845</v>
       </c>
       <c r="S56" s="68">
-        <v>2.0923396021910001</v>
+        <v>2.6391529445950002</v>
       </c>
       <c r="T56" s="68">
-        <v>3.1393377807039999</v>
+        <v>3.2080107949590002</v>
+      </c>
+      <c r="U56" s="10">
+        <v>3.2895803722610002</v>
+      </c>
+      <c r="V56" s="16">
+        <v>0.34188854248200001</v>
+      </c>
+      <c r="W56" s="35">
+        <v>0.48888964209000002</v>
+      </c>
+      <c r="X56" s="35">
+        <v>0.62304656269600001</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.2">
@@ -9121,25 +9181,37 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N57" s="8">
-        <v>4.5753599609000002E-2</v>
+        <v>5.3802480419000001E-2</v>
       </c>
       <c r="O57" s="5">
-        <v>4.3814211659999998E-2</v>
+        <v>5.1333357088999998E-2</v>
       </c>
       <c r="P57" s="5">
-        <v>2.2989321404590002</v>
+        <v>1.530615660117</v>
       </c>
       <c r="Q57" s="5">
-        <v>1.801042356807</v>
+        <v>1.388551751182</v>
       </c>
       <c r="R57" s="68">
-        <v>10.983961607873001</v>
+        <v>11.160036264612</v>
       </c>
       <c r="S57" s="68">
-        <v>0.90216369038199995</v>
+        <v>1.1157244378169999</v>
       </c>
       <c r="T57" s="68">
-        <v>1.3170759723600001</v>
+        <v>1.374698045775</v>
+      </c>
+      <c r="U57" s="10">
+        <v>4.4807277071409999</v>
+      </c>
+      <c r="V57" s="16">
+        <v>0.30646791229300002</v>
+      </c>
+      <c r="W57" s="35">
+        <v>0.40227830299099998</v>
+      </c>
+      <c r="X57" s="35">
+        <v>0.50886283933599996</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.2">
@@ -9183,25 +9255,37 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N58" s="8">
-        <v>2.8175569740000002E-3</v>
+        <v>5.0722943560000001E-3</v>
       </c>
       <c r="O58" s="5">
-        <v>2.8266037849999999E-3</v>
+        <v>5.0848720279999997E-3</v>
       </c>
       <c r="P58" s="5">
-        <v>2.8735446417819999</v>
+        <v>1.8291973798329999</v>
       </c>
       <c r="Q58" s="5">
-        <v>1.9722087181700001</v>
+        <v>1.6625538060559999</v>
       </c>
       <c r="R58" s="68">
-        <v>4916.6786699054301</v>
+        <v>6646.7809369616198</v>
       </c>
       <c r="S58" s="68">
-        <v>132.92945143268801</v>
+        <v>195.953452813708</v>
       </c>
       <c r="T58" s="68">
-        <v>225.40543365478501</v>
+        <v>219.41810186734401</v>
+      </c>
+      <c r="U58" s="10">
+        <v>1.664115735917</v>
+      </c>
+      <c r="V58" s="16">
+        <v>0.48827158859300002</v>
+      </c>
+      <c r="W58" s="35">
+        <v>0.67023641358499997</v>
+      </c>
+      <c r="X58" s="35">
+        <v>0.86726488241800004</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.2">
@@ -9245,25 +9329,37 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N59" s="8">
-        <v>2.7243058779E-2</v>
+        <v>3.4714399745999998E-2</v>
       </c>
       <c r="O59" s="5">
-        <v>2.7102555702999999E-2</v>
+        <v>3.4400825147999997E-2</v>
       </c>
       <c r="P59" s="5">
-        <v>2.490143377011</v>
+        <v>1.615903268594</v>
       </c>
       <c r="Q59" s="5">
-        <v>1.8649202338069999</v>
+        <v>1.4593310582929999</v>
       </c>
       <c r="R59" s="68">
-        <v>162.42864808014099</v>
+        <v>178.110285268025</v>
       </c>
       <c r="S59" s="68">
-        <v>8.0666463323070001</v>
+        <v>10.180519812041</v>
       </c>
       <c r="T59" s="68">
-        <v>12.309307266375001</v>
+        <v>12.184290868039</v>
+      </c>
+      <c r="U59" s="10">
+        <v>2.6903158978059998</v>
+      </c>
+      <c r="V59" s="16">
+        <v>0.38428085230800002</v>
+      </c>
+      <c r="W59" s="35">
+        <v>0.53094029280300004</v>
+      </c>
+      <c r="X59" s="35">
+        <v>0.67849427514399996</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.2">
@@ -9307,25 +9403,37 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="N60" s="8">
-        <v>4.1814717132000002E-2</v>
+        <v>4.9427278024000001E-2</v>
       </c>
       <c r="O60" s="5">
-        <v>4.1413592397000001E-2</v>
+        <v>4.8730297972E-2</v>
       </c>
       <c r="P60" s="5">
-        <v>2.3772578897379999</v>
+        <v>1.5623064079919999</v>
       </c>
       <c r="Q60" s="5">
-        <v>1.831500762611</v>
+        <v>1.4148099488749999</v>
       </c>
       <c r="R60" s="68">
-        <v>35.753100829746998</v>
+        <v>37.236168857734</v>
       </c>
       <c r="S60" s="68">
-        <v>2.4733025538760001</v>
+        <v>3.0142100131610001</v>
       </c>
       <c r="T60" s="68">
-        <v>3.6590898437499999</v>
+        <v>3.6133512209499998</v>
+      </c>
+      <c r="U60" s="10">
+        <v>3.5656139495630002</v>
+      </c>
+      <c r="V60" s="16">
+        <v>0.34104787539300002</v>
+      </c>
+      <c r="W60" s="35">
+        <v>0.45378575776699998</v>
+      </c>
+      <c r="X60" s="35">
+        <v>0.57524149968899996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>